<commit_message>
aded: daily hours to met productivity target column
</commit_message>
<xml_diff>
--- a/SampleOutputReport.xlsx
+++ b/SampleOutputReport.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="39">
   <si>
     <t>Dzień</t>
   </si>
@@ -128,10 +128,13 @@
     <t>Udział w godzinach</t>
   </si>
   <si>
-    <t>"Idealne" godziny</t>
+    <t>Godziny wg obrotu</t>
   </si>
   <si>
     <t>Różnica godzin</t>
+  </si>
+  <si>
+    <t>Godziny wg celu produktywności: 800.0</t>
   </si>
 </sst>
 </file>
@@ -206,13 +209,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -249,13 +252,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -292,13 +295,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -335,13 +338,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -378,13 +381,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -421,13 +424,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -464,13 +467,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>150586</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -505,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -516,8 +519,9 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="37.2421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -543,6 +547,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>38</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -567,6 +574,9 @@
       <c r="G4" t="n" s="2">
         <v>-15.359691731313944</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>324.1335435595357</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -590,6 +600,9 @@
       <c r="G5" t="n" s="2">
         <v>39.694777460374894</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>207.1666628265878</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -613,6 +626,9 @@
       <c r="G6" t="n" s="2">
         <v>9.120148013437927</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>172.87273464330738</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -636,6 +652,9 @@
       <c r="G7" t="n" s="2">
         <v>47.91523119638373</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>190.12297852454026</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -659,6 +678,9 @@
       <c r="G8" t="n" s="2">
         <v>101.10854222100812</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>187.66693474764162</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -682,6 +704,9 @@
       <c r="G9" t="n" s="2">
         <v>15.932206249243563</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>295.5880173238273</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -705,6 +730,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -728,6 +756,9 @@
       <c r="G11" t="n" s="2">
         <v>49.66439522601624</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>220.41418510629052</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -751,6 +782,9 @@
       <c r="G12" t="n" s="2">
         <v>-11.202725728780479</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>264.4970221275486</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -774,6 +808,9 @@
       <c r="G13" t="n" s="2">
         <v>-64.04146994991865</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>327.4725035864887</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -797,6 +834,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -820,6 +860,9 @@
       <c r="G15" t="n" s="2">
         <v>-78.22796301528462</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>403.0430813372169</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -843,6 +886,9 @@
       <c r="G16" t="n" s="2">
         <v>-101.95904519284517</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>415.6381776290049</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -866,6 +912,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -889,6 +938,9 @@
       <c r="G18" t="n" s="2">
         <v>46.74952542699185</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>277.0921184193366</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -912,6 +964,9 @@
       <c r="G19" t="n" s="2">
         <v>13.152685159024713</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>201.52154066860845</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -935,6 +990,9 @@
       <c r="G20" t="n" s="2">
         <v>3.283767336585356</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>188.9264443768204</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -958,6 +1016,9 @@
       <c r="G21" t="n" s="2">
         <v>30.067100669918375</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>188.9264443768204</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -981,6 +1042,9 @@
       <c r="G22" t="n" s="2">
         <v>38.4450231154471</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>251.90192583576058</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -1004,6 +1068,9 @@
       <c r="G23" t="n" s="2">
         <v>-97.63246532682928</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>377.8528887536408</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -1027,6 +1094,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -1050,6 +1120,9 @@
       <c r="G25" t="n" s="2">
         <v>53.29502311544712</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>251.90192583576058</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -1073,6 +1146,9 @@
       <c r="G26" t="n" s="2">
         <v>41.5360184923577</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>201.52154066860845</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -1096,6 +1172,9 @@
       <c r="G27" t="n" s="2">
         <v>20.283767336585356</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>188.9264443768204</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -1119,6 +1198,9 @@
       <c r="G28" t="n" s="2">
         <v>10.58826964813008</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>214.11663696039645</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -1142,6 +1224,9 @@
       <c r="G29" t="n" s="2">
         <v>-22.693721105691054</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>314.8774072947006</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -1165,6 +1250,9 @@
       <c r="G30" t="n" s="2">
         <v>-62.53246532682931</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>377.8528887536408</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -1188,6 +1276,9 @@
       <c r="G31" t="n" s="2">
         <v>-84.15588546081338</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>340.0675998782768</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -1211,6 +1302,9 @@
       <c r="G32" t="n" s="2">
         <v>14.380607604552523</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>264.4970221275486</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -1234,6 +1328,9 @@
       <c r="G33" t="n" s="2">
         <v>2.9450231154471282</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>251.90192583576058</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -1256,6 +1353,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>6900.9</v>
       </c>
     </row>
     <row r="35"/>
@@ -1293,7 +1393,7 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2070,7 +2170,7 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2847,7 +2947,7 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -3624,7 +3724,7 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -4401,7 +4501,7 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -5178,7 +5278,7 @@
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added: 8 column for departments with hours to met store productivity target
</commit_message>
<xml_diff>
--- a/SampleOutputReport.xlsx
+++ b/SampleOutputReport.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="40">
   <si>
     <t>Dzień</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Godziny wg celu produktywności: 800.0</t>
+  </si>
+  <si>
+    <t>Godziny wg celu produktywności</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1385,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1395,6 +1398,7 @@
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="31.08984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -1420,6 +1424,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -1444,6 +1451,9 @@
       <c r="G4" t="n" s="2">
         <v>6.342984928757964</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>31.115956058551163</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -1467,6 +1477,9 @@
       <c r="G5" t="n" s="2">
         <v>7.214481684607165</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>23.482640995498347</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -1490,6 +1503,9 @@
       <c r="G6" t="n" s="2">
         <v>-5.6839309520855075</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>17.04385233544235</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -1513,6 +1529,9 @@
       <c r="G7" t="n" s="2">
         <v>1.1523206812383826</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>23.555477971290834</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -1536,6 +1555,9 @@
       <c r="G8" t="n" s="2">
         <v>6.460389410430729</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>32.150241114804494</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -1559,6 +1581,9 @@
       <c r="G9" t="n" s="2">
         <v>5.923533481791516</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>37.42363816218067</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -1582,6 +1607,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -1605,6 +1633,9 @@
       <c r="G11" t="n" s="2">
         <v>-7.647193645467269</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>26.221311285295922</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -1628,6 +1659,9 @@
       <c r="G12" t="n" s="2">
         <v>2.823367625439282</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>23.307832253596374</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -1651,6 +1685,9 @@
       <c r="G13" t="n" s="2">
         <v>-1.675830558979932</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>25.114189253250093</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -1674,6 +1711,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -1697,6 +1737,9 @@
       <c r="G15" t="n" s="2">
         <v>-16.554868380283004</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>30.766338574747213</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -1720,6 +1763,9 @@
       <c r="G16" t="n" s="2">
         <v>-5.634708017166844</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>35.576006876244605</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -1743,6 +1789,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -1766,6 +1815,9 @@
       <c r="G18" t="n" s="2">
         <v>9.243527988555435</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>33.35933491295981</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -1789,6 +1841,9 @@
       <c r="G19" t="n" s="2">
         <v>-11.277434190141502</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>18.2262392424738</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -1812,6 +1867,9 @@
       <c r="G20" t="n" s="2">
         <v>-7.697594553257655</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>16.89817838385737</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -1835,6 +1893,9 @@
       <c r="G21" t="n" s="2">
         <v>-7.697594553257655</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>20.799812387141635</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -1858,6 +1919,9 @@
       <c r="G22" t="n" s="2">
         <v>0.40320726232312154</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>29.120222921836966</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -1881,6 +1945,9 @@
       <c r="G23" t="n" s="2">
         <v>0.6048108934846894</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>30.28561453451679</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -1904,6 +1971,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -1927,6 +1997,9 @@
       <c r="G25" t="n" s="2">
         <v>8.403207262323122</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>29.171208804891712</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -1950,6 +2023,9 @@
       <c r="G26" t="n" s="2">
         <v>4.722565809858498</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>22.870810398841442</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -1973,6 +2049,9 @@
       <c r="G27" t="n" s="2">
         <v>3.3024054467423447</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>18.209243948122168</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -1996,6 +2075,9 @@
       <c r="G28" t="n" s="2">
         <v>2.1427261729746583</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>22.404653753769516</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -2019,6 +2101,9 @@
       <c r="G29" t="n" s="2">
         <v>0.504009077903909</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>30.66436680863773</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -2042,6 +2127,9 @@
       <c r="G30" t="n" s="2">
         <v>9.10481089348469</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>36.345650920451845</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -2065,6 +2153,9 @@
       <c r="G31" t="n" s="2">
         <v>3.3443298041362155</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>28.406420559070582</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -2088,6 +2179,9 @@
       <c r="G32" t="n" s="2">
         <v>6.823367625439282</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>25.638615478956012</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -2111,6 +2205,9 @@
       <c r="G33" t="n" s="2">
         <v>-14.596792737676878</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>22.71056905209797</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -2133,6 +2230,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>690.8684269885267</v>
       </c>
     </row>
     <row r="35"/>
@@ -2159,7 +2259,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2172,6 +2272,7 @@
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="31.08984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -2197,6 +2298,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -2221,6 +2325,9 @@
       <c r="G4" t="n" s="2">
         <v>-15.454274179942722</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>48.32533957696773</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -2244,6 +2351,9 @@
       <c r="G5" t="n" s="2">
         <v>4.813739607826964</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>36.47024690920972</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -2267,6 +2377,9 @@
       <c r="G6" t="n" s="2">
         <v>5.824254423783042</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>26.47034049861996</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -2290,6 +2403,9 @@
       <c r="G7" t="n" s="2">
         <v>3.0099305322252903</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>36.58336802245169</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -2313,6 +2429,9 @@
       <c r="G8" t="n" s="2">
         <v>15.225535934425757</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>49.931659385003634</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -2336,6 +2455,9 @@
       <c r="G9" t="n" s="2">
         <v>8.051613427991338</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>58.12162798372194</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -2359,6 +2481,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -2382,6 +2507,9 @@
       <c r="G11" t="n" s="2">
         <v>5.650797238419514</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>40.723600767107634</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -2405,6 +2533,9 @@
       <c r="G12" t="n" s="2">
         <v>2.780956686103419</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>36.19875623742901</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -2428,6 +2559,9 @@
       <c r="G13" t="n" s="2">
         <v>-13.747386960062432</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>39.00415984582976</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -2451,6 +2585,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -2474,6 +2611,9 @@
       <c r="G15" t="n" s="2">
         <v>-14.38139933546146</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>47.78235823340629</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -2497,6 +2637,9 @@
       <c r="G16" t="n" s="2">
         <v>-15.487068064694625</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>55.25212241115084</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -2520,6 +2663,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -2543,6 +2689,9 @@
       <c r="G18" t="n" s="2">
         <v>2.675287956870246</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>51.809469864820265</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -2566,6 +2715,9 @@
       <c r="G19" t="n" s="2">
         <v>-0.2906996677307312</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>28.306673236914616</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -2589,6 +2741,9 @@
       <c r="G20" t="n" s="2">
         <v>-4.585030938497557</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>26.244098272136032</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -2612,6 +2767,9 @@
       <c r="G21" t="n" s="2">
         <v>-4.585030938497557</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>32.30361923813059</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -2635,6 +2793,9 @@
       <c r="G22" t="n" s="2">
         <v>9.886625415336585</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>45.22582107413786</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -2658,6 +2819,9 @@
       <c r="G23" t="n" s="2">
         <v>-13.170061876995113</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>47.03575888600932</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -2681,6 +2845,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -2704,6 +2871,9 @@
       <c r="G25" t="n" s="2">
         <v>-3.113374584663415</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>45.305005853407245</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -2727,6 +2897,9 @@
       <c r="G26" t="n" s="2">
         <v>2.3093003322692702</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>35.52002955797722</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -2750,6 +2923,9 @@
       <c r="G27" t="n" s="2">
         <v>9.414969061502443</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>28.28027831049141</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -2773,6 +2949,9 @@
       <c r="G28" t="n" s="2">
         <v>7.203631603036101</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>34.79605443322864</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -2796,6 +2975,9 @@
       <c r="G29" t="n" s="2">
         <v>-1.6417182308292588</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>47.62398867486754</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -2819,6 +3001,9 @@
       <c r="G30" t="n" s="2">
         <v>7.829938123004887</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>56.447435507740856</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -2842,6 +3027,9 @@
       <c r="G31" t="n" s="2">
         <v>11.146944310704392</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>44.11723416436661</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -2865,6 +3053,9 @@
       <c r="G32" t="n" s="2">
         <v>-1.2190433138965808</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>39.81863186117191</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -2888,6 +3079,9 @@
       <c r="G33" t="n" s="2">
         <v>-8.113374584663415</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>35.27116310884489</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -2910,6 +3104,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>1072.968841915142</v>
       </c>
     </row>
     <row r="35"/>
@@ -2936,7 +3133,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2949,6 +3146,7 @@
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="31.08984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -2974,6 +3172,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -2998,6 +3199,9 @@
       <c r="G4" t="n" s="2">
         <v>0.4105652258577379</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>28.682305864027605</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -3021,6 +3225,9 @@
       <c r="G5" t="n" s="2">
         <v>-0.3857656743195683</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>21.646009856185625</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -3044,6 +3251,9 @@
       <c r="G6" t="n" s="2">
         <v>-4.514535826795992</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>15.710813605296018</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -3067,6 +3277,9 @@
       <c r="G7" t="n" s="2">
         <v>3.5381906315673497</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>21.713150085268087</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -3090,6 +3303,9 @@
       <c r="G8" t="n" s="2">
         <v>8.815438251762405</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>29.635697116998557</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -3113,6 +3329,9 @@
       <c r="G9" t="n" s="2">
         <v>2.6328934638581245</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>34.496649702568774</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -3136,6 +3355,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -3159,6 +3381,9 @@
       <c r="G11" t="n" s="2">
         <v>11.118803315828323</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>24.17048246968618</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -3182,6 +3407,9 @@
       <c r="G12" t="n" s="2">
         <v>-3.8574360210060057</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>21.48487330638772</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -3205,6 +3433,9 @@
       <c r="G13" t="n" s="2">
         <v>-9.966349359340768</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>23.149950987632767</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -3228,6 +3459,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -3251,6 +3485,9 @@
       <c r="G15" t="n" s="2">
         <v>-1.4970453653424869</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>28.360032764431786</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -3274,6 +3511,9 @@
       <c r="G16" t="n" s="2">
         <v>0.08117196699056706</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>32.793525891510384</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -3297,6 +3537,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -3320,6 +3563,9 @@
       <c r="G18" t="n" s="2">
         <v>8.720781311327041</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>30.75022491976742</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -3343,6 +3589,9 @@
       <c r="G19" t="n" s="2">
         <v>1.2514773173287566</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>16.800723324068024</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -3366,6 +3615,9 @@
       <c r="G20" t="n" s="2">
         <v>-0.3267400150042903</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>15.576533147131094</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -3389,6 +3641,9 @@
       <c r="G21" t="n" s="2">
         <v>2.6732599849957097</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>19.173011418314914</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -3412,6 +3667,9 @@
       <c r="G22" t="n" s="2">
         <v>-1.435653353339056</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>26.84266358716815</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -3435,6 +3693,9 @@
       <c r="G23" t="n" s="2">
         <v>-5.653480030008581</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>27.91690725248754</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -3458,6 +3719,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -3481,6 +3745,9 @@
       <c r="G25" t="n" s="2">
         <v>5.564346646660944</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>26.889661747525878</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -3504,6 +3771,9 @@
       <c r="G26" t="n" s="2">
         <v>1.2514773173287566</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>21.08203193189295</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -3527,6 +3797,9 @@
       <c r="G27" t="n" s="2">
         <v>-7.32674001500429</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>16.785057270615404</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -3550,6 +3823,9 @@
       <c r="G28" t="n" s="2">
         <v>-0.1703053503381966</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>20.652334465765193</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -3573,6 +3849,9 @@
       <c r="G29" t="n" s="2">
         <v>-6.544566691673815</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>28.26603644371634</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -3596,6 +3875,9 @@
       <c r="G30" t="n" s="2">
         <v>-1.6534800300085806</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>33.502974312148346</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -3619,6 +3901,9 @@
       <c r="G31" t="n" s="2">
         <v>-8.388132027007728</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>26.18468934216003</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -3642,6 +3927,9 @@
       <c r="G32" t="n" s="2">
         <v>3.1425639789939943</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>23.633360637026488</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -3665,6 +3953,9 @@
       <c r="G33" t="n" s="2">
         <v>2.564346646660944</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>20.934323427911533</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -3687,6 +3978,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>636.8340248776922</v>
       </c>
     </row>
     <row r="35"/>
@@ -3713,7 +4007,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3726,6 +4020,7 @@
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="31.08984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -3751,6 +4046,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -3775,6 +4073,9 @@
       <c r="G4" t="n" s="2">
         <v>5.342844573706476</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>20.488727155537056</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -3798,6 +4099,9 @@
       <c r="G5" t="n" s="2">
         <v>7.405790429231857</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>15.462466373935264</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -3821,6 +4125,9 @@
       <c r="G6" t="n" s="2">
         <v>3.6493741538514186</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>11.22275785204979</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -3844,6 +4151,9 @@
       <c r="G7" t="n" s="2">
         <v>9.017813896308098</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>15.510426877576503</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -3867,6 +4177,9 @@
       <c r="G8" t="n" s="2">
         <v>21.250111100032505</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>21.169766307242636</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -3890,6 +4203,9 @@
       <c r="G9" t="n" s="2">
         <v>13.94273371483979</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>24.642106770868295</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -3913,6 +4229,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -3936,6 +4255,9 @@
       <c r="G11" t="n" s="2">
         <v>6.152815050373743</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>17.26578131084583</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -3959,6 +4281,9 @@
       <c r="G12" t="n" s="2">
         <v>-6.016621939551502</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>15.347361165196293</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -3982,6 +4307,9 @@
       <c r="G13" t="n" s="2">
         <v>-3.972960496587575</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>16.536781655499006</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -4005,6 +4333,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -4028,6 +4359,9 @@
       <c r="G15" t="n" s="2">
         <v>-8.120566765030865</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>20.258516738059107</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -4051,6 +4385,9 @@
       <c r="G16" t="n" s="2">
         <v>-8.31183447643808</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>23.425508661835586</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -4074,6 +4411,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -4097,6 +4437,9 @@
       <c r="G18" t="n" s="2">
         <v>12.79211034904128</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>21.965910667687197</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -4120,6 +4463,9 @@
       <c r="G19" t="n" s="2">
         <v>0.9397166174845673</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>12.001316694492594</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -4143,6 +4489,9 @@
       <c r="G20" t="n" s="2">
         <v>1.1309843288917847</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>11.126836844767313</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -4166,6 +4515,9 @@
       <c r="G21" t="n" s="2">
         <v>9.130984328891785</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>13.695921156482955</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -4189,6 +4541,9 @@
       <c r="G22" t="n" s="2">
         <v>-8.825354228144292</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>19.174609355767117</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -4212,6 +4567,9 @@
       <c r="G23" t="n" s="2">
         <v>-16.838031342216432</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>19.941977414026933</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -4235,6 +4593,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -4258,6 +4619,9 @@
       <c r="G25" t="n" s="2">
         <v>14.074645771855707</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>19.208181708315987</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -4281,6 +4645,9 @@
       <c r="G26" t="n" s="2">
         <v>3.9397166174845673</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>15.059598143348863</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -4304,6 +4671,9 @@
       <c r="G27" t="n" s="2">
         <v>-5.869015671108215</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>11.990125910309605</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -4327,6 +4697,9 @@
       <c r="G28" t="n" s="2">
         <v>-1.2515510939226466</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>14.752650920044939</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -4350,6 +4723,9 @@
       <c r="G29" t="n" s="2">
         <v>1.2183072148196423</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>20.191372032961375</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -4373,6 +4749,9 @@
       <c r="G30" t="n" s="2">
         <v>-15.73803134221643</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>23.932291316977967</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -4396,6 +4775,9 @@
       <c r="G31" t="n" s="2">
         <v>-22.164228207994796</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>18.704596420082982</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -4419,6 +4801,9 @@
       <c r="G32" t="n" s="2">
         <v>-6.016621939551502</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>16.88209728171592</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -4442,6 +4827,9 @@
       <c r="G33" t="n" s="2">
         <v>-6.825354228144292</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>14.954085035338139</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -4464,6 +4852,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>454.9117717709648</v>
       </c>
     </row>
     <row r="35"/>
@@ -4490,7 +4881,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4503,6 +4894,7 @@
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="31.08984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -4528,6 +4920,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -4552,6 +4947,9 @@
       <c r="G4" t="n" s="2">
         <v>0.5233509416867754</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>21.20752312370526</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -4575,6 +4973,9 @@
       <c r="G5" t="n" s="2">
         <v>4.160299086417762</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>16.00492849972513</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -4598,6 +4999,9 @@
       <c r="G6" t="n" s="2">
         <v>-1.7210169452755704</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>11.616480362703724</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -4621,6 +5025,9 @@
       <c r="G7" t="n" s="2">
         <v>4.710248824155599</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>16.05457157819822</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -4644,6 +5051,9 @@
       <c r="G8" t="n" s="2">
         <v>10.93360102549973</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>21.912454838023177</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -4667,6 +5077,9 @@
       <c r="G9" t="n" s="2">
         <v>8.119276219257749</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>25.506613719475098</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -4690,6 +5103,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -4713,6 +5129,9 @@
       <c r="G11" t="n" s="2">
         <v>10.955571674244645</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>17.871508250313422</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -4736,6 +5155,9 @@
       <c r="G12" t="n" s="2">
         <v>-3.053313990906421</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>15.885785111389708</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -4759,6 +5181,9 @@
       <c r="G13" t="n" s="2">
         <v>-7.780293512550806</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>17.11693345752241</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -4782,6 +5207,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -4805,6 +5233,9 @@
       <c r="G15" t="n" s="2">
         <v>-21.652668938524073</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>20.969236347034414</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -4828,6 +5259,9 @@
       <c r="G16" t="n" s="2">
         <v>-1.0813981761859424</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>24.247334295541016</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -4851,6 +5285,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -4874,6 +5311,9 @@
       <c r="G18" t="n" s="2">
         <v>5.8012901047647</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>22.73652994067652</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -4897,6 +5337,9 @@
       <c r="G19" t="n" s="2">
         <v>-1.6096678025950375</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>12.422353003250299</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -4920,6 +5363,9 @@
       <c r="G20" t="n" s="2">
         <v>1.8190614350668426</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>11.517194205757537</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -4943,6 +5389,9 @@
       <c r="G21" t="n" s="2">
         <v>2.6023947683998436</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>14.176408442632846</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -4966,6 +5415,9 @@
       <c r="G22" t="n" s="2">
         <v>-4.907918086577546</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>19.847302773542513</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -4989,6 +5441,9 @@
       <c r="G23" t="n" s="2">
         <v>-2.361877129866315</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>20.641592029112</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -5012,6 +5467,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -5035,6 +5493,9 @@
       <c r="G25" t="n" s="2">
         <v>3.442081913422456</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>19.88205292847368</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -5058,6 +5519,9 @@
       <c r="G26" t="n" s="2">
         <v>1.6736655307379635</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>15.587926640551151</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -5081,6 +5545,9 @@
       <c r="G27" t="n" s="2">
         <v>-0.1809385649331574</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>12.410769618273209</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -5104,6 +5571,9 @@
       <c r="G28" t="n" s="2">
         <v>0.528269626409088</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>15.270210938323357</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -5127,6 +5597,9 @@
       <c r="G29" t="n" s="2">
         <v>-4.634897608221927</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>20.899736037172083</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -5150,6 +5623,9 @@
       <c r="G30" t="n" s="2">
         <v>-9.361877129866315</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>24.77189615807332</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -5173,6 +5649,9 @@
       <c r="G31" t="n" s="2">
         <v>-14.925689416879688</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>19.360800604506206</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -5196,6 +5675,9 @@
       <c r="G32" t="n" s="2">
         <v>12.946686009093579</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>17.474363622528678</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -5219,6 +5701,9 @@
       <c r="G33" t="n" s="2">
         <v>5.092081913422454</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>15.478711867910347</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -5241,6 +5726,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>470.8712183944148</v>
       </c>
     </row>
     <row r="35"/>
@@ -5267,7 +5755,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5280,6 +5768,7 @@
     <col min="5" max="5" width="18.578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.40625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="31.08984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -5305,6 +5794,9 @@
       <c r="G2" t="s" s="4">
         <v>37</v>
       </c>
+      <c r="H2" t="s" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -5329,6 +5821,9 @@
       <c r="G4" t="n" s="2">
         <v>-6.322639284702198</v>
       </c>
+      <c r="H4" t="n" s="2">
+        <v>44.32719997167903</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -5352,6 +5847,9 @@
       <c r="G5" t="n" s="2">
         <v>-4.38152685585095</v>
       </c>
+      <c r="H5" t="n" s="2">
+        <v>33.452924323195965</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -5375,6 +5873,9 @@
       <c r="G6" t="n" s="2">
         <v>0.6409936219588417</v>
       </c>
+      <c r="H6" t="n" s="2">
+        <v>24.28034829909385</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -5398,6 +5899,9 @@
       <c r="G7" t="n" s="2">
         <v>9.61159592605452</v>
       </c>
+      <c r="H7" t="n" s="2">
+        <v>33.55668649541432</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -5421,6 +5925,9 @@
       <c r="G8" t="n" s="2">
         <v>29.042913501040893</v>
       </c>
+      <c r="H8" t="n" s="2">
+        <v>45.800622817179594</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -5444,6 +5951,9 @@
       <c r="G9" t="n" s="2">
         <v>15.090376879139484</v>
       </c>
+      <c r="H9" t="n" s="2">
+        <v>53.313004085788116</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -5467,6 +5977,9 @@
       <c r="G10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -5490,6 +6003,9 @@
       <c r="G11" t="n" s="2">
         <v>2.2920125012225228</v>
       </c>
+      <c r="H11" t="n" s="2">
+        <v>37.35438199860592</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -5513,6 +6029,9 @@
       <c r="G12" t="n" s="2">
         <v>-14.449584998532963</v>
       </c>
+      <c r="H12" t="n" s="2">
+        <v>33.20389510987193</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -5536,6 +6055,9 @@
       <c r="G13" t="n" s="2">
         <v>-15.509009998183672</v>
       </c>
+      <c r="H13" t="n" s="2">
+        <v>35.777196980887005</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -5559,6 +6081,9 @@
       <c r="G14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -5582,6 +6107,9 @@
       <c r="G15" t="n" s="2">
         <v>-3.5803199977645193</v>
       </c>
+      <c r="H15" t="n" s="2">
+        <v>43.82914154503094</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -5605,6 +6133,9 @@
       <c r="G16" t="n" s="2">
         <v>-10.992204997694657</v>
       </c>
+      <c r="H16" t="n" s="2">
+        <v>50.68090365051606</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -5628,6 +6159,9 @@
       <c r="G17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -5651,6 +6185,9 @@
       <c r="G18" t="n" s="2">
         <v>-0.6614699984631116</v>
       </c>
+      <c r="H18" t="n" s="2">
+        <v>47.5230748760042</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -5674,6 +6211,9 @@
       <c r="G19" t="n" s="2">
         <v>-2.390159998882261</v>
       </c>
+      <c r="H19" t="n" s="2">
+        <v>25.964754228105132</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -5697,6 +6237,9 @@
       <c r="G20" t="n" s="2">
         <v>-4.178274998952119</v>
       </c>
+      <c r="H20" t="n" s="2">
+        <v>24.07282395465715</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -5720,6 +6263,9 @@
       <c r="G21" t="n" s="2">
         <v>10.82172500104788</v>
       </c>
+      <c r="H21" t="n" s="2">
+        <v>29.631017646486686</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -5743,6 +6289,9 @@
       <c r="G22" t="n" s="2">
         <v>31.662300001397178</v>
       </c>
+      <c r="H22" t="n" s="2">
+        <v>41.48411645289624</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -5766,6 +6315,9 @@
       <c r="G23" t="n" s="2">
         <v>-14.356549997904239</v>
       </c>
+      <c r="H23" t="n" s="2">
+        <v>43.144311208389844</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -5789,6 +6341,9 @@
       <c r="G24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="H24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -5812,6 +6367,9 @@
       <c r="G25" t="n" s="2">
         <v>-1.237699998602828</v>
       </c>
+      <c r="H25" t="n" s="2">
+        <v>41.55674997344909</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -5835,6 +6393,9 @@
       <c r="G26" t="n" s="2">
         <v>4.609840001117739</v>
       </c>
+      <c r="H26" t="n" s="2">
+        <v>32.58132207656183</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -5858,6 +6419,9 @@
       <c r="G27" t="n" s="2">
         <v>-4.178274998952119</v>
       </c>
+      <c r="H27" t="n" s="2">
+        <v>25.940543054587447</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -5881,6 +6445,9 @@
       <c r="G28" t="n" s="2">
         <v>-1.8020449988124057</v>
       </c>
+      <c r="H28" t="n" s="2">
+        <v>31.917244174364395</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -5904,6 +6471,9 @@
       <c r="G29" t="n" s="2">
         <v>5.202875001746477</v>
       </c>
+      <c r="H29" t="n" s="2">
+        <v>43.68387450392526</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -5927,6 +6497,9 @@
       <c r="G30" t="n" s="2">
         <v>-0.3565499979042386</v>
       </c>
+      <c r="H30" t="n" s="2">
+        <v>51.777323936956535</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -5950,6 +6523,9 @@
       <c r="G31" t="n" s="2">
         <v>-7.72089499811382</v>
       </c>
+      <c r="H31" t="n" s="2">
+        <v>40.467247165156415</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -5973,6 +6549,9 @@
       <c r="G32" t="n" s="2">
         <v>-21.449584998532963</v>
       </c>
+      <c r="H32" t="n" s="2">
+        <v>36.52428462085912</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -5996,6 +6575,9 @@
       <c r="G33" t="n" s="2">
         <v>4.6623000013971705</v>
       </c>
+      <c r="H33" t="n" s="2">
+        <v>32.35304529768146</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -6018,6 +6600,9 @@
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="3">
+        <v>984.1980384473425</v>
       </c>
     </row>
     <row r="35"/>

</xml_diff>

<commit_message>
added: styling for drop area
</commit_message>
<xml_diff>
--- a/SampleOutputReport.xlsx
+++ b/SampleOutputReport.xlsx
@@ -588,19 +588,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>242.0</v>
+        <v>241.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>0.03564327270049341</v>
+        <v>0.03451485857500895</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>202.66731216377482</v>
+        <v>208.42838311857395</v>
       </c>
       <c r="G4" t="n" s="2">
         <v>208.5720389179112</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>-33.427961082088814</v>
+        <v>-32.427961082088814</v>
       </c>
     </row>
     <row r="5">
@@ -614,19 +614,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>207.5</v>
+        <v>214.5</v>
       </c>
       <c r="E5" t="n" s="5">
-        <v>0.03056189704691067</v>
+        <v>0.030719656283566057</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>202.66731216377482</v>
+        <v>208.42838311857395</v>
       </c>
       <c r="G5" t="n" s="2">
         <v>208.5720389179112</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>1.0720389179111862</v>
+        <v>-5.927961082088814</v>
       </c>
     </row>
     <row r="6">
@@ -640,19 +640,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>284.0</v>
+        <v>291.0</v>
       </c>
       <c r="E6" t="n" s="5">
-        <v>0.04182929523528978</v>
+        <v>0.04167561761546724</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G6" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>-52.253290091209834</v>
+        <v>-59.253290091209834</v>
       </c>
     </row>
     <row r="7">
@@ -669,10 +669,10 @@
         <v>231.0</v>
       </c>
       <c r="E7" t="n" s="5">
-        <v>0.03402312394138007</v>
+        <v>0.03308270676691729</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>315.260263365872</v>
+        <v>324.2219292955595</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>324.4453938723063</v>
@@ -718,19 +718,19 @@
         <v>0.036315615714757346</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>238.0</v>
+        <v>251.0</v>
       </c>
       <c r="E9" t="n" s="5">
-        <v>0.03505412769717947</v>
+        <v>0.03594701038310061</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>247.70449264461368</v>
+        <v>254.74580158936814</v>
       </c>
       <c r="G9" t="n" s="2">
         <v>254.9213808996692</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>16.921380899669202</v>
+        <v>3.9213808996692023</v>
       </c>
     </row>
     <row r="10">
@@ -744,19 +744,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>223.75</v>
+        <v>233.0</v>
       </c>
       <c r="E10" t="n" s="5">
-        <v>0.03295529862287355</v>
+        <v>0.03336913712853563</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G10" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>7.996709908790166</v>
+        <v>-1.2532900912098341</v>
       </c>
     </row>
     <row r="11">
@@ -770,19 +770,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>241.25</v>
+        <v>246.0</v>
       </c>
       <c r="E11" t="n" s="5">
-        <v>0.03553280801237205</v>
+        <v>0.03523093447905478</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G11" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>-9.503290091209834</v>
+        <v>-14.253290091209834</v>
       </c>
     </row>
     <row r="12">
@@ -796,19 +796,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>244.5</v>
+        <v>261.5</v>
       </c>
       <c r="E12" t="n" s="5">
-        <v>0.03601148832756462</v>
+        <v>0.03745076978159685</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>202.66731216377482</v>
+        <v>208.42838311857395</v>
       </c>
       <c r="G12" t="n" s="2">
         <v>208.5720389179112</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>-35.927961082088814</v>
+        <v>-52.927961082088814</v>
       </c>
     </row>
     <row r="13">
@@ -822,19 +822,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>300.0</v>
+        <v>309.0</v>
       </c>
       <c r="E13" t="n" s="5">
-        <v>0.04418587524854555</v>
+        <v>0.044253490870032226</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>270.2230828850331</v>
+        <v>277.9045108247652</v>
       </c>
       <c r="G13" t="n" s="2">
         <v>278.0960518905482</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>-21.90394810945179</v>
+        <v>-30.90394810945179</v>
       </c>
     </row>
     <row r="14">
@@ -848,19 +848,19 @@
         <v>0.05117200396170353</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>263.0</v>
+        <v>251.0</v>
       </c>
       <c r="E14" t="n" s="5">
-        <v>0.0387362839678916</v>
+        <v>0.03594701038310061</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>349.03814872650105</v>
+        <v>358.9599931486551</v>
       </c>
       <c r="G14" t="n" s="2">
         <v>359.2074003586248</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>96.2074003586248</v>
+        <v>108.2074003586248</v>
       </c>
     </row>
     <row r="15">
@@ -900,19 +900,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>305.0</v>
+        <v>306.0</v>
       </c>
       <c r="E16" t="n" s="5">
-        <v>0.04492230650268798</v>
+        <v>0.04382384532760473</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>281.4823780052429</v>
+        <v>289.4838654424638</v>
       </c>
       <c r="G16" t="n" s="2">
         <v>289.68338738598777</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>-15.316612614012229</v>
+        <v>-16.31661261401223</v>
       </c>
     </row>
     <row r="17">
@@ -926,19 +926,19 @@
         <v>0.034664905909541105</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>248.0</v>
+        <v>257.0</v>
       </c>
       <c r="E17" t="n" s="5">
-        <v>0.03652699020546432</v>
+        <v>0.036806301467955604</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>236.445197524404</v>
+        <v>243.16644697166961</v>
       </c>
       <c r="G17" t="n" s="2">
         <v>243.33404540422973</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>-4.665954595770273</v>
+        <v>-13.665954595770273</v>
       </c>
     </row>
     <row r="18">
@@ -952,19 +952,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>256.0</v>
+        <v>257.0</v>
       </c>
       <c r="E18" t="n" s="5">
-        <v>0.0377052802120922</v>
+        <v>0.036806301467955604</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G18" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>-24.253290091209834</v>
+        <v>-25.253290091209834</v>
       </c>
     </row>
     <row r="19">
@@ -978,19 +978,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D19" t="n" s="2">
-        <v>262.5</v>
+        <v>259.5</v>
       </c>
       <c r="E19" t="n" s="5">
-        <v>0.03866264084247736</v>
+        <v>0.037164339419978515</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G19" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>-30.753290091209834</v>
+        <v>-27.753290091209834</v>
       </c>
     </row>
     <row r="20">
@@ -1004,19 +1004,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>278.0</v>
+        <v>291.0</v>
       </c>
       <c r="E20" t="n" s="5">
-        <v>0.04094557773031887</v>
+        <v>0.04167561761546724</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>270.2230828850331</v>
+        <v>277.9045108247652</v>
       </c>
       <c r="G20" t="n" s="2">
         <v>278.0960518905482</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>0.0960518905482104</v>
+        <v>-12.90394810945179</v>
       </c>
     </row>
     <row r="21">
@@ -1030,19 +1030,19 @@
         <v>0.04621987454605481</v>
       </c>
       <c r="D21" t="n" s="2">
-        <v>271.0</v>
+        <v>265.0</v>
       </c>
       <c r="E21" t="n" s="5">
-        <v>0.03991457397451948</v>
+        <v>0.03795202291442893</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>315.260263365872</v>
+        <v>324.2219292955595</v>
       </c>
       <c r="G21" t="n" s="2">
         <v>324.4453938723063</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>53.44539387230628</v>
+        <v>59.44539387230628</v>
       </c>
     </row>
     <row r="22">
@@ -1082,19 +1082,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D23" t="n" s="2">
-        <v>239.0</v>
+        <v>256.0</v>
       </c>
       <c r="E23" t="n" s="5">
-        <v>0.03520141394800795</v>
+        <v>0.036663086287146436</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>281.4823780052429</v>
+        <v>289.4838654424638</v>
       </c>
       <c r="G23" t="n" s="2">
         <v>289.68338738598777</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>50.68338738598777</v>
+        <v>33.68338738598777</v>
       </c>
     </row>
     <row r="24">
@@ -1108,19 +1108,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D24" t="n" s="2">
-        <v>203.0</v>
+        <v>220.0</v>
       </c>
       <c r="E24" t="n" s="5">
-        <v>0.02989910891818249</v>
+        <v>0.03150733977801647</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G24" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>28.746709908790166</v>
+        <v>11.746709908790166</v>
       </c>
     </row>
     <row r="25">
@@ -1134,19 +1134,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D25" t="n" s="2">
-        <v>206.0</v>
+        <v>223.0</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>0.030340967670667945</v>
+        <v>0.031936985320443964</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G25" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>25.746709908790166</v>
+        <v>8.746709908790166</v>
       </c>
     </row>
     <row r="26">
@@ -1160,19 +1160,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D26" t="n" s="2">
-        <v>235.5</v>
+        <v>252.5</v>
       </c>
       <c r="E26" t="n" s="5">
-        <v>0.03468591207010826</v>
+        <v>0.03616183315431436</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G26" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>-3.753290091209834</v>
+        <v>-20.753290091209834</v>
       </c>
     </row>
     <row r="27">
@@ -1186,19 +1186,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D27" t="n" s="2">
-        <v>266.0</v>
+        <v>283.0</v>
       </c>
       <c r="E27" t="n" s="5">
-        <v>0.039178142720377056</v>
+        <v>0.04052989616899391</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>270.2230828850331</v>
+        <v>277.9045108247652</v>
       </c>
       <c r="G27" t="n" s="2">
         <v>278.0960518905482</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>12.09605189054821</v>
+        <v>-4.90394810945179</v>
       </c>
     </row>
     <row r="28">
@@ -1212,19 +1212,19 @@
         <v>0.04621987454605481</v>
       </c>
       <c r="D28" t="n" s="2">
-        <v>258.0</v>
+        <v>254.0</v>
       </c>
       <c r="E28" t="n" s="5">
-        <v>0.03799985271374917</v>
+        <v>0.036376655925528106</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>315.260263365872</v>
+        <v>324.2219292955595</v>
       </c>
       <c r="G28" t="n" s="2">
         <v>324.4453938723063</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>66.44539387230628</v>
+        <v>70.44539387230628</v>
       </c>
     </row>
     <row r="29">
@@ -1264,19 +1264,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D30" t="n" s="2">
-        <v>272.0</v>
+        <v>283.0</v>
       </c>
       <c r="E30" t="n" s="5">
-        <v>0.04006186022534797</v>
+        <v>0.04052989616899391</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>281.4823780052429</v>
+        <v>289.4838654424638</v>
       </c>
       <c r="G30" t="n" s="2">
         <v>289.68338738598777</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>17.68338738598777</v>
+        <v>6.683387385987771</v>
       </c>
     </row>
     <row r="31">
@@ -1290,19 +1290,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D31" t="n" s="2">
-        <v>251.0</v>
+        <v>248.0</v>
       </c>
       <c r="E31" t="n" s="5">
-        <v>0.036968848957949774</v>
+        <v>0.03551736484067311</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G31" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>-19.253290091209834</v>
+        <v>-16.253290091209834</v>
       </c>
     </row>
     <row r="32">
@@ -1316,19 +1316,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D32" t="n" s="2">
-        <v>242.0</v>
+        <v>251.0</v>
       </c>
       <c r="E32" t="n" s="5">
-        <v>0.03564327270049341</v>
+        <v>0.03594701038310061</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G32" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>-10.253290091209834</v>
+        <v>-19.253290091209834</v>
       </c>
     </row>
     <row r="33">
@@ -1342,19 +1342,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D33" t="n" s="2">
-        <v>254.5</v>
+        <v>263.5</v>
       </c>
       <c r="E33" t="n" s="5">
-        <v>0.03748435083584947</v>
+        <v>0.03773720014321518</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>225.18590240419422</v>
+        <v>231.587092353971</v>
       </c>
       <c r="G33" t="n" s="2">
         <v>231.74670990879017</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>-22.753290091209834</v>
+        <v>-31.753290091209834</v>
       </c>
     </row>
     <row r="34">
@@ -1368,19 +1368,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D34" t="n" s="2">
-        <v>267.0</v>
+        <v>284.0</v>
       </c>
       <c r="E34" t="n" s="5">
-        <v>0.039325428971205535</v>
+        <v>0.04067311134980308</v>
       </c>
       <c r="F34" t="n" s="2">
-        <v>270.2230828850331</v>
+        <v>277.9045108247652</v>
       </c>
       <c r="G34" t="n" s="2">
         <v>278.0960518905482</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>11.09605189054821</v>
+        <v>-5.90394810945179</v>
       </c>
     </row>
     <row r="35">
@@ -1394,19 +1394,19 @@
         <v>1.0</v>
       </c>
       <c r="D35" t="n" s="3">
-        <v>6789.5</v>
+        <v>6982.5</v>
       </c>
       <c r="E35" t="n" s="3">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="3">
-        <v>6789.354957486456</v>
+        <v>6982.3508344722295</v>
       </c>
       <c r="G35" t="n" s="3">
         <v>6987.312572087659</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>197.81257208765874</v>
+        <v>4.812572087658737</v>
       </c>
     </row>
     <row r="36"/>
@@ -1500,16 +1500,16 @@
         <v>36.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>0.03748047891723061</v>
+        <v>0.036566785170137124</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>28.67102928541214</v>
+        <v>29.387431891190268</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>24.256471987635745</v>
+        <v>24.113786858296713</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>-11.743528012364255</v>
+        <v>-11.886213141703287</v>
       </c>
     </row>
     <row r="5">
@@ -1526,16 +1526,16 @@
         <v>36.5</v>
       </c>
       <c r="E5" t="n" s="5">
-        <v>0.03800104112441437</v>
+        <v>0.03707465718638903</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>28.67102928541214</v>
+        <v>29.387431891190268</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>20.47531606015135</v>
+        <v>21.474111965524585</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>-16.02468393984865</v>
+        <v>-15.025888034475415</v>
       </c>
     </row>
     <row r="6">
@@ -1552,16 +1552,16 @@
         <v>45.0</v>
       </c>
       <c r="E6" t="n" s="5">
-        <v>0.04685059864653826</v>
+        <v>0.0457084814626714</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>31.390728454587435</v>
+        <v>32.389524359960674</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>-13.609271545412565</v>
+        <v>-12.610475640039326</v>
       </c>
     </row>
     <row r="7">
@@ -1578,10 +1578,10 @@
         <v>38.0</v>
       </c>
       <c r="E7" t="n" s="5">
-        <v>0.03956272774596564</v>
+        <v>0.038598273235144746</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>44.59937888841889</v>
+        <v>45.713782941851534</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>29.25045151450193</v>
@@ -1630,16 +1630,16 @@
         <v>38.0</v>
       </c>
       <c r="E9" t="n" s="5">
-        <v>0.03956272774596564</v>
+        <v>0.038598273235144746</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>35.04236912661484</v>
+        <v>35.91797231145477</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>27.110174574416423</v>
+        <v>28.96508125582386</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>-10.889825425583577</v>
+        <v>-9.034918744176139</v>
       </c>
     </row>
     <row r="10">
@@ -1656,16 +1656,16 @@
         <v>36.0</v>
       </c>
       <c r="E10" t="n" s="5">
-        <v>0.03748047891723061</v>
+        <v>0.036566785170137124</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>22.79394941191065</v>
+        <v>24.113786858296713</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>-13.20605058808935</v>
+        <v>-11.886213141703287</v>
       </c>
     </row>
     <row r="11">
@@ -1682,16 +1682,16 @@
         <v>30.0</v>
       </c>
       <c r="E11" t="n" s="5">
-        <v>0.031233732431025507</v>
+        <v>0.03047232097511427</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>25.148254046004705</v>
+        <v>25.826008410365116</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>-4.8517459539952945</v>
+        <v>-4.173991589634884</v>
       </c>
     </row>
     <row r="12">
@@ -1705,19 +1705,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>35.5</v>
+        <v>43.5</v>
       </c>
       <c r="E12" t="n" s="5">
-        <v>0.03695991671004685</v>
+        <v>0.04418486541391569</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>28.67102928541214</v>
+        <v>29.387431891190268</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>26.753461751068837</v>
+        <v>29.17910894983241</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>-8.746538248931163</v>
+        <v>-14.320891050167589</v>
       </c>
     </row>
     <row r="13">
@@ -1734,16 +1734,16 @@
         <v>38.0</v>
       </c>
       <c r="E13" t="n" s="5">
-        <v>0.03956272774596564</v>
+        <v>0.038598273235144746</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>38.228039047216186</v>
+        <v>39.18324252158702</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>32.817579747977774</v>
+        <v>34.101745912029074</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>-5.182420252022226</v>
+        <v>-3.898254087970926</v>
       </c>
     </row>
     <row r="14">
@@ -1760,16 +1760,16 @@
         <v>39.0</v>
       </c>
       <c r="E14" t="n" s="5">
-        <v>0.04060385216033316</v>
+        <v>0.03961401726764855</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>49.3778837693209</v>
+        <v>50.6116882570499</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>32.817579747977774</v>
+        <v>31.105358195909368</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>-6.182420252022226</v>
+        <v>-7.894641804090632</v>
       </c>
     </row>
     <row r="15">
@@ -1812,16 +1812,16 @@
         <v>46.0</v>
       </c>
       <c r="E16" t="n" s="5">
-        <v>0.04789172306090578</v>
+        <v>0.046724225495175215</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>39.82087400751686</v>
+        <v>40.815877626653155</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>33.10295000665584</v>
+        <v>33.245635135994874</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>-12.897049993344162</v>
+        <v>-12.754364864005126</v>
       </c>
     </row>
     <row r="17">
@@ -1838,16 +1838,16 @@
         <v>39.0</v>
       </c>
       <c r="E17" t="n" s="5">
-        <v>0.04060385216033316</v>
+        <v>0.03961401726764855</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>33.449534166314166</v>
+        <v>34.28533720638865</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>26.111378669043184</v>
+        <v>27.39554483309449</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>-12.888621330956816</v>
+        <v>-11.60445516690551</v>
       </c>
     </row>
     <row r="18">
@@ -1864,16 +1864,16 @@
         <v>29.0</v>
       </c>
       <c r="E18" t="n" s="5">
-        <v>0.03019260801665799</v>
+        <v>0.029456576942610464</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>26.111378669043184</v>
+        <v>26.25406379838222</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>-2.8886213309568163</v>
+        <v>-2.7459362016177806</v>
       </c>
     </row>
     <row r="19">
@@ -1890,16 +1890,16 @@
         <v>33.5</v>
       </c>
       <c r="E19" t="n" s="5">
-        <v>0.034877667881311816</v>
+        <v>0.0340274250888776</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>28.180313044459176</v>
+        <v>27.752257656442072</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>-5.319686955540824</v>
+        <v>-5.747742343557928</v>
       </c>
     </row>
     <row r="20">
@@ -1916,16 +1916,16 @@
         <v>30.0</v>
       </c>
       <c r="E20" t="n" s="5">
-        <v>0.031233732431025507</v>
+        <v>0.03047232097511427</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>38.228039047216186</v>
+        <v>39.18324252158702</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>31.676098713265503</v>
+        <v>32.389524359960674</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>1.6760987132655032</v>
+        <v>2.3895243599606744</v>
       </c>
     </row>
     <row r="21">
@@ -1942,16 +1942,16 @@
         <v>44.0</v>
       </c>
       <c r="E21" t="n" s="5">
-        <v>0.045809474232170744</v>
+        <v>0.0446927374301676</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>44.59937888841889</v>
+        <v>45.713782941851534</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>33.959060782690045</v>
+        <v>33.10295000665584</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>-10.040939217309955</v>
+        <v>-10.897049993344162</v>
       </c>
     </row>
     <row r="22">
@@ -1994,16 +1994,16 @@
         <v>30.0</v>
       </c>
       <c r="E23" t="n" s="5">
-        <v>0.031233732431025507</v>
+        <v>0.03047232097511427</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>39.82087400751686</v>
+        <v>40.815877626653155</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>27.110174574416423</v>
+        <v>28.394340738467726</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>-2.8898254255835774</v>
+        <v>-1.6056592615322742</v>
       </c>
     </row>
     <row r="24">
@@ -2020,16 +2020,16 @@
         <v>30.0</v>
       </c>
       <c r="E24" t="n" s="5">
-        <v>0.031233732431025507</v>
+        <v>0.03047232097511427</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G24" t="n" s="2">
-        <v>20.974714012837968</v>
+        <v>22.25888017688927</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>-9.025285987162032</v>
+        <v>-7.741119823110729</v>
       </c>
     </row>
     <row r="25">
@@ -2046,16 +2046,16 @@
         <v>38.0</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>0.03956272774596564</v>
+        <v>0.038598273235144746</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>21.402769400855068</v>
+        <v>22.686935564906374</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>-16.597230599144932</v>
+        <v>-15.313064435093626</v>
       </c>
     </row>
     <row r="26">
@@ -2072,16 +2072,16 @@
         <v>33.5</v>
       </c>
       <c r="E26" t="n" s="5">
-        <v>0.034877667881311816</v>
+        <v>0.0340274250888776</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>25.611980716356566</v>
+        <v>26.89614688040787</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>-7.888019283643434</v>
+        <v>-6.603853119592131</v>
       </c>
     </row>
     <row r="27">
@@ -2098,16 +2098,16 @@
         <v>31.0</v>
       </c>
       <c r="E27" t="n" s="5">
-        <v>0.032274856845393024</v>
+        <v>0.03148806500761808</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>38.228039047216186</v>
+        <v>39.18324252158702</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>29.963877161197097</v>
+        <v>31.2480433252484</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>-1.0361228388029033</v>
+        <v>0.24804332524839978</v>
       </c>
     </row>
     <row r="28">
@@ -2124,16 +2124,16 @@
         <v>43.0</v>
       </c>
       <c r="E28" t="n" s="5">
-        <v>0.04476834981780323</v>
+        <v>0.04367699339766379</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>44.59937888841889</v>
+        <v>45.713782941851534</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>32.24683923062164</v>
+        <v>31.676098713265503</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>-10.753160769378361</v>
+        <v>-11.323901286734497</v>
       </c>
     </row>
     <row r="29">
@@ -2173,19 +2173,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D30" t="n" s="2">
-        <v>30.0</v>
+        <v>38.0</v>
       </c>
       <c r="E30" t="n" s="5">
-        <v>0.031233732431025507</v>
+        <v>0.038598273235144746</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>39.82087400751686</v>
+        <v>40.815877626653155</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>28.394340738467726</v>
+        <v>29.963877161197097</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>-1.6056592615322742</v>
+        <v>-8.036122838802903</v>
       </c>
     </row>
     <row r="31">
@@ -2202,16 +2202,16 @@
         <v>30.0</v>
       </c>
       <c r="E31" t="n" s="5">
-        <v>0.031233732431025507</v>
+        <v>0.03047232097511427</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>25.397953022348016</v>
+        <v>24.969897634330913</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>-4.602046977651984</v>
+        <v>-5.030102365669087</v>
       </c>
     </row>
     <row r="32">
@@ -2228,16 +2228,16 @@
         <v>34.0</v>
       </c>
       <c r="E32" t="n" s="5">
-        <v>0.035398230088495575</v>
+        <v>0.03453529710512951</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>25.25526789300898</v>
+        <v>26.539434057060287</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>-8.74473210699102</v>
+        <v>-7.460565942939713</v>
       </c>
     </row>
     <row r="33">
@@ -2254,16 +2254,16 @@
         <v>34.5</v>
       </c>
       <c r="E33" t="n" s="5">
-        <v>0.03591879229567933</v>
+        <v>0.03504316912138141</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>31.856699206013484</v>
+        <v>32.65270210132251</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>27.181517139085937</v>
+        <v>28.465683303137244</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>-7.318482860914063</v>
+        <v>-6.034316696862756</v>
       </c>
     </row>
     <row r="34">
@@ -2277,19 +2277,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D34" t="n" s="2">
-        <v>33.0</v>
+        <v>41.0</v>
       </c>
       <c r="E34" t="n" s="5">
-        <v>0.03435710567412806</v>
+        <v>0.04164550533265617</v>
       </c>
       <c r="F34" t="n" s="2">
-        <v>38.228039047216186</v>
+        <v>39.18324252158702</v>
       </c>
       <c r="G34" t="n" s="2">
-        <v>28.108970479789658</v>
+        <v>30.534617678553232</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>-4.891029520210342</v>
+        <v>-10.465382321446768</v>
       </c>
     </row>
     <row r="35">
@@ -2303,19 +2303,19 @@
         <v>1.0</v>
       </c>
       <c r="D35" t="n" s="3">
-        <v>960.5</v>
+        <v>984.5</v>
       </c>
       <c r="E35" t="n" s="3">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="3">
-        <v>960.4794810613063</v>
+        <v>984.4789683548734</v>
       </c>
       <c r="G35" t="n" s="3">
-        <v>743.6035515503746</v>
+        <v>764.2928953045346</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>-216.89644844962538</v>
+        <v>-220.20710469546543</v>
       </c>
     </row>
     <row r="36">
@@ -2413,16 +2413,16 @@
         <v>28.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>0.0307776861775213</v>
+        <v>0.03160270880361174</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>27.15613627527714</v>
+        <v>26.447196196642537</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>52.79349785544251</v>
+        <v>52.48294786805755</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>24.79349785544251</v>
+        <v>24.48294786805755</v>
       </c>
     </row>
     <row r="5">
@@ -2439,16 +2439,16 @@
         <v>12.0</v>
       </c>
       <c r="E5" t="n" s="5">
-        <v>0.013190436933223413</v>
+        <v>0.013544018058690745</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>27.15613627527714</v>
+        <v>26.447196196642537</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>44.563923189741175</v>
+        <v>46.73777310143587</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>32.563923189741175</v>
+        <v>34.73777310143587</v>
       </c>
     </row>
     <row r="6">
@@ -2465,16 +2465,16 @@
         <v>38.0</v>
       </c>
       <c r="E6" t="n" s="5">
-        <v>0.041769716955207474</v>
+        <v>0.04288939051918736</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>68.3209972246903</v>
+        <v>70.49484713638499</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>30.320997224690302</v>
+        <v>32.49484713638499</v>
       </c>
     </row>
     <row r="7">
@@ -2491,10 +2491,10 @@
         <v>38.0</v>
       </c>
       <c r="E7" t="n" s="5">
-        <v>0.041769716955207474</v>
+        <v>0.04288939051918736</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>42.24287865043111</v>
+        <v>41.14008297255506</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>63.662747413915966</v>
@@ -2543,16 +2543,16 @@
         <v>25.0</v>
       </c>
       <c r="E9" t="n" s="5">
-        <v>0.027480076944215445</v>
+        <v>0.028216704288939052</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>33.19083322533873</v>
+        <v>32.32435090700754</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>59.00449760314163</v>
+        <v>63.041647439146054</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>34.00449760314163</v>
+        <v>38.041647439146054</v>
       </c>
     </row>
     <row r="10">
@@ -2566,19 +2566,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>35.75</v>
+        <v>32.0</v>
       </c>
       <c r="E10" t="n" s="5">
-        <v>0.039296510030228084</v>
+        <v>0.03611738148984198</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>49.61036048474671</v>
+        <v>52.48294786805755</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>13.860360484746707</v>
+        <v>20.48294786805755</v>
       </c>
     </row>
     <row r="11">
@@ -2595,16 +2595,16 @@
         <v>34.0</v>
       </c>
       <c r="E11" t="n" s="5">
-        <v>0.037372904644133</v>
+        <v>0.03837471783295711</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>54.73443527659848</v>
+        <v>56.20954771667702</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>20.734435276598482</v>
+        <v>22.209547716677022</v>
       </c>
     </row>
     <row r="12">
@@ -2621,16 +2621,16 @@
         <v>28.0</v>
       </c>
       <c r="E12" t="n" s="5">
-        <v>0.0307776861775213</v>
+        <v>0.03160270880361174</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>27.15613627527714</v>
+        <v>26.447196196642537</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>58.22812263467924</v>
+        <v>63.507472420223486</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>30.228122634679238</v>
+        <v>35.507472420223486</v>
       </c>
     </row>
     <row r="13">
@@ -2647,16 +2647,16 @@
         <v>44.0</v>
       </c>
       <c r="E13" t="n" s="5">
-        <v>0.04836493542181918</v>
+        <v>0.04966139954853273</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>36.208181700369515</v>
+        <v>35.262928262190044</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>71.42649709853987</v>
+        <v>74.22144698500446</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>27.42649709853987</v>
+        <v>30.221446985004462</v>
       </c>
     </row>
     <row r="14">
@@ -2673,16 +2673,16 @@
         <v>42.0</v>
       </c>
       <c r="E14" t="n" s="5">
-        <v>0.046166529266281946</v>
+        <v>0.04740406320541761</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>46.768901362977296</v>
+        <v>45.54794900532881</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>71.42649709853987</v>
+        <v>67.6998972499204</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>29.42649709853987</v>
+        <v>25.699897249920397</v>
       </c>
     </row>
     <row r="15">
@@ -2725,16 +2725,16 @@
         <v>35.0</v>
       </c>
       <c r="E16" t="n" s="5">
-        <v>0.03847210772190162</v>
+        <v>0.039503386004514675</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>37.71685593788492</v>
+        <v>36.7322169397813</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>72.04759707330977</v>
+        <v>72.35814706069473</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>37.047597073309774</v>
+        <v>37.35814706069473</v>
       </c>
     </row>
     <row r="17">
@@ -2751,16 +2751,16 @@
         <v>28.0</v>
       </c>
       <c r="E17" t="n" s="5">
-        <v>0.0307776861775213</v>
+        <v>0.03160270880361174</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>31.682158987823335</v>
+        <v>30.855062229416294</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>56.830647691446934</v>
+        <v>59.625597577911535</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>28.830647691446934</v>
+        <v>31.625597577911535</v>
       </c>
     </row>
     <row r="18">
@@ -2777,16 +2777,16 @@
         <v>36.0</v>
       </c>
       <c r="E18" t="n" s="5">
-        <v>0.03957131079967024</v>
+        <v>0.040632054176072234</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>56.830647691446934</v>
+        <v>57.141197678831894</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>20.830647691446934</v>
+        <v>21.141197678831894</v>
       </c>
     </row>
     <row r="19">
@@ -2803,16 +2803,16 @@
         <v>34.0</v>
       </c>
       <c r="E19" t="n" s="5">
-        <v>0.037372904644133</v>
+        <v>0.03837471783295711</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>61.3336225085288</v>
+        <v>60.401972546373926</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>27.333622508528798</v>
+        <v>26.401972546373926</v>
       </c>
     </row>
     <row r="20">
@@ -2826,19 +2826,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>38.0</v>
+        <v>34.0</v>
       </c>
       <c r="E20" t="n" s="5">
-        <v>0.041769716955207474</v>
+        <v>0.03837471783295711</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>36.208181700369515</v>
+        <v>35.262928262190044</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>68.94209719946022</v>
+        <v>70.49484713638499</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>30.94209719946022</v>
+        <v>36.49484713638499</v>
       </c>
     </row>
     <row r="21">
@@ -2852,19 +2852,19 @@
         <v>0.04621987454605481</v>
       </c>
       <c r="D21" t="n" s="2">
-        <v>46.0</v>
+        <v>40.0</v>
       </c>
       <c r="E21" t="n" s="5">
-        <v>0.05056334157735642</v>
+        <v>0.045146726862302484</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>42.24287865043111</v>
+        <v>41.14008297255506</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>73.91089699761952</v>
+        <v>72.04759707330977</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>27.910896997619517</v>
+        <v>32.047597073309774</v>
       </c>
     </row>
     <row r="22">
@@ -2907,16 +2907,16 @@
         <v>32.0</v>
       </c>
       <c r="E23" t="n" s="5">
-        <v>0.035174498488595766</v>
+        <v>0.03611738148984198</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>37.71685593788492</v>
+        <v>36.7322169397813</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>59.00449760314163</v>
+        <v>61.79944748960623</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>27.00449760314163</v>
+        <v>29.79944748960623</v>
       </c>
     </row>
     <row r="24">
@@ -2933,16 +2933,16 @@
         <v>28.0</v>
       </c>
       <c r="E24" t="n" s="5">
-        <v>0.0307776861775213</v>
+        <v>0.03160270880361174</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G24" t="n" s="2">
-        <v>45.65084814558852</v>
+        <v>48.445798032053126</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>17.65084814558852</v>
+        <v>20.445798032053126</v>
       </c>
     </row>
     <row r="25">
@@ -2959,16 +2959,16 @@
         <v>32.0</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>0.035174498488595766</v>
+        <v>0.03611738148984198</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>46.58249810774339</v>
+        <v>49.37744799420799</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>14.58249810774339</v>
+        <v>17.37744799420799</v>
       </c>
     </row>
     <row r="26">
@@ -2985,16 +2985,16 @@
         <v>28.0</v>
       </c>
       <c r="E26" t="n" s="5">
-        <v>0.0307776861775213</v>
+        <v>0.03160270880361174</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>55.74372273559959</v>
+        <v>58.53867262206419</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>27.74372273559959</v>
+        <v>30.53867262206419</v>
       </c>
     </row>
     <row r="27">
@@ -3011,16 +3011,16 @@
         <v>36.0</v>
       </c>
       <c r="E27" t="n" s="5">
-        <v>0.03957131079967024</v>
+        <v>0.040632054176072234</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>36.208181700369515</v>
+        <v>35.262928262190044</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>65.21549735084075</v>
+        <v>68.01044723730534</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>29.21549735084075</v>
+        <v>32.01044723730534</v>
       </c>
     </row>
     <row r="28">
@@ -3034,19 +3034,19 @@
         <v>0.04621987454605481</v>
       </c>
       <c r="D28" t="n" s="2">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="E28" t="n" s="5">
-        <v>0.04396812311074471</v>
+        <v>0.040632054176072234</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>42.24287865043111</v>
+        <v>41.14008297255506</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>70.18429714900005</v>
+        <v>68.94209719946022</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>30.184297149000045</v>
+        <v>32.94209719946022</v>
       </c>
     </row>
     <row r="29">
@@ -3086,19 +3086,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D30" t="n" s="2">
-        <v>34.0</v>
+        <v>28.0</v>
       </c>
       <c r="E30" t="n" s="5">
-        <v>0.037372904644133</v>
+        <v>0.03160270880361174</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>37.71685593788492</v>
+        <v>36.7322169397813</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>61.79944748960623</v>
+        <v>65.21549735084075</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>27.79944748960623</v>
+        <v>37.21549735084075</v>
       </c>
     </row>
     <row r="31">
@@ -3115,16 +3115,16 @@
         <v>34.0</v>
       </c>
       <c r="E31" t="n" s="5">
-        <v>0.037372904644133</v>
+        <v>0.03837471783295711</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>55.27789775452216</v>
+        <v>54.346247792367286</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>21.277897754522158</v>
+        <v>20.346247792367286</v>
       </c>
     </row>
     <row r="32">
@@ -3141,16 +3141,16 @@
         <v>36.0</v>
       </c>
       <c r="E32" t="n" s="5">
-        <v>0.03957131079967024</v>
+        <v>0.040632054176072234</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>54.9673477671372</v>
+        <v>57.762297653601806</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>18.9673477671372</v>
+        <v>21.762297653601806</v>
       </c>
     </row>
     <row r="33">
@@ -3167,16 +3167,16 @@
         <v>36.0</v>
       </c>
       <c r="E33" t="n" s="5">
-        <v>0.03957131079967024</v>
+        <v>0.040632054176072234</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>30.173484750307928</v>
+        <v>29.385773551825036</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>59.1597725968341</v>
+        <v>61.95472248329871</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>23.159772596834102</v>
+        <v>25.95472248329871</v>
       </c>
     </row>
     <row r="34">
@@ -3193,16 +3193,16 @@
         <v>32.0</v>
       </c>
       <c r="E34" t="n" s="5">
-        <v>0.035174498488595766</v>
+        <v>0.03611738148984198</v>
       </c>
       <c r="F34" t="n" s="2">
-        <v>36.208181700369515</v>
+        <v>35.262928262190044</v>
       </c>
       <c r="G34" t="n" s="2">
-        <v>61.17834751483632</v>
+        <v>66.45769730038057</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>29.178347514836318</v>
+        <v>34.45769730038057</v>
       </c>
     </row>
     <row r="35">
@@ -3216,19 +3216,19 @@
         <v>1.0</v>
       </c>
       <c r="D35" t="n" s="3">
-        <v>909.75</v>
+        <v>886.0</v>
       </c>
       <c r="E35" t="n" s="3">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="3">
-        <v>909.7305652217841</v>
+        <v>885.9810725875252</v>
       </c>
       <c r="G35" t="n" s="3">
-        <v>1618.4312592566978</v>
+        <v>1663.4610074275165</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>708.6812592566978</v>
+        <v>777.4610074275165</v>
       </c>
     </row>
     <row r="36">
@@ -3332,10 +3332,10 @@
         <v>26.506896413790713</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>28.679710997145794</v>
+        <v>28.51100681480964</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>1.6797109971457935</v>
+        <v>1.5110068148096403</v>
       </c>
     </row>
     <row r="5">
@@ -3358,10 +3358,10 @@
         <v>26.506896413790713</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>24.209050165237773</v>
+        <v>25.389979441590835</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>-0.7909498347622268</v>
+        <v>0.3899794415908353</v>
       </c>
     </row>
     <row r="6">
@@ -3384,10 +3384,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>37.11492011395338</v>
+        <v>38.295849390306444</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>5.1149201139533815</v>
+        <v>6.295849390306444</v>
       </c>
     </row>
     <row r="7">
@@ -3462,10 +3462,10 @@
         <v>32.39731783907754</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>32.05379464386883</v>
+        <v>34.2469490142388</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>-8.946205356131173</v>
+        <v>-6.753050985761199</v>
       </c>
     </row>
     <row r="10">
@@ -3488,10 +3488,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>26.95049312820024</v>
+        <v>28.51100681480964</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>-3.0495068717997604</v>
+        <v>-1.4889931851903597</v>
       </c>
     </row>
     <row r="11">
@@ -3514,10 +3514,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>29.73411213674674</v>
+        <v>30.53545700284346</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>-0.2658878632532584</v>
+        <v>0.5354570028434615</v>
       </c>
     </row>
     <row r="12">
@@ -3540,10 +3540,10 @@
         <v>26.506896413790713</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>31.63203418802845</v>
+        <v>34.50000528774303</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>-1.3679658119715512</v>
+        <v>1.5000052877430292</v>
       </c>
     </row>
     <row r="13">
@@ -3566,10 +3566,10 @@
         <v>35.342528551720946</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>38.8019619373149</v>
+        <v>40.32029957834026</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>15.8019619373149</v>
+        <v>17.32029957834026</v>
       </c>
     </row>
     <row r="14">
@@ -3592,10 +3592,10 @@
         <v>45.650766045972894</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>38.8019619373149</v>
+        <v>36.777511749281075</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>-0.19803806268510016</v>
+        <v>-2.222488250718925</v>
       </c>
     </row>
     <row r="15">
@@ -3644,10 +3644,10 @@
         <v>36.81513390804266</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>39.1393703019872</v>
+        <v>39.30807448432335</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>-3.8606296980128008</v>
+        <v>-3.691925515676651</v>
       </c>
     </row>
     <row r="17">
@@ -3670,10 +3670,10 @@
         <v>30.924712482755837</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>30.872865367515764</v>
+        <v>32.39120300854113</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>-2.1271346324842355</v>
+        <v>-0.6087969914588669</v>
       </c>
     </row>
     <row r="18">
@@ -3696,10 +3696,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>30.872865367515764</v>
+        <v>31.041569549851918</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>5.8728653675157645</v>
+        <v>6.041569549851918</v>
       </c>
     </row>
     <row r="19">
@@ -3722,10 +3722,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>33.31907601138997</v>
+        <v>32.81296346438151</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>2.319076011389967</v>
+        <v>1.812963464381511</v>
       </c>
     </row>
     <row r="20">
@@ -3748,10 +3748,10 @@
         <v>35.342528551720946</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>37.45232847862568</v>
+        <v>38.295849390306444</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>6.452328478625681</v>
+        <v>7.295849390306444</v>
       </c>
     </row>
     <row r="21">
@@ -3774,10 +3774,10 @@
         <v>41.23294997700778</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>40.15159539600411</v>
+        <v>39.1393703019872</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>-6.848404603995888</v>
+        <v>-7.860629698012801</v>
       </c>
     </row>
     <row r="22">
@@ -3826,10 +3826,10 @@
         <v>36.81513390804266</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>32.05379464386883</v>
+        <v>33.572132284894195</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>-11.946205356131173</v>
+        <v>-10.427867715105805</v>
       </c>
     </row>
     <row r="24">
@@ -3852,10 +3852,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G24" t="n" s="2">
-        <v>24.799514803414304</v>
+        <v>26.31785244443967</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>-7.200485196585696</v>
+        <v>-5.682147555560331</v>
       </c>
     </row>
     <row r="25">
@@ -3878,10 +3878,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>25.30562735042276</v>
+        <v>26.823964991448126</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>4.3056273504227605</v>
+        <v>5.8239649914481255</v>
       </c>
     </row>
     <row r="26">
@@ -3904,10 +3904,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>30.282400729339233</v>
+        <v>31.800738370364602</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>-1.7175992706607666</v>
+        <v>-0.19926162963539795</v>
       </c>
     </row>
     <row r="27">
@@ -3930,10 +3930,10 @@
         <v>35.342528551720946</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>35.42787829059186</v>
+        <v>36.946215931617225</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>3.427878290591863</v>
+        <v>4.946215931617225</v>
       </c>
     </row>
     <row r="28">
@@ -3956,10 +3956,10 @@
         <v>41.23294997700778</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>38.12714520797029</v>
+        <v>37.45232847862568</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>0.12714520797028683</v>
+        <v>-0.5476715213743191</v>
       </c>
     </row>
     <row r="29">
@@ -4008,10 +4008,10 @@
         <v>36.81513390804266</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>33.572132284894195</v>
+        <v>35.42787829059186</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>-10.427867715105805</v>
+        <v>-8.572121709408137</v>
       </c>
     </row>
     <row r="31">
@@ -4034,10 +4034,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>30.02934445583501</v>
+        <v>29.523231908826553</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>0.029344455835008887</v>
+        <v>-0.4767680911734473</v>
       </c>
     </row>
     <row r="32">
@@ -4060,10 +4060,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>29.860640273498856</v>
+        <v>31.37897791452422</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>-2.1393597265011444</v>
+        <v>-0.6210220854757793</v>
       </c>
     </row>
     <row r="33">
@@ -4086,10 +4086,10 @@
         <v>29.45210712643412</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>32.138146735036905</v>
+        <v>33.65648437606227</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>2.138146735036905</v>
+        <v>3.6564843760622665</v>
       </c>
     </row>
     <row r="34">
@@ -4112,10 +4112,10 @@
         <v>35.342528551720946</v>
       </c>
       <c r="G34" t="n" s="2">
-        <v>33.23472392022189</v>
+        <v>36.10269501993647</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>0.2347239202218887</v>
+        <v>3.102695019936469</v>
       </c>
     </row>
     <row r="35">
@@ -4138,10 +4138,10 @@
         <v>887.9810298619891</v>
       </c>
       <c r="G35" t="n" s="3">
-        <v>879.2018462448547</v>
+        <v>903.6639526835967</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>-8.798153755145336</v>
+        <v>15.663952683596676</v>
       </c>
     </row>
     <row r="36">
@@ -4236,19 +4236,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>0.04898958971218616</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>13.788187446518148</v>
+        <v>14.95490439561841</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>17.869115098722162</v>
+        <v>17.764002656964973</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>-2.130884901277838</v>
+        <v>-1.2359973430350273</v>
       </c>
     </row>
     <row r="5">
@@ -4262,19 +4262,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>20.0</v>
+        <v>27.0</v>
       </c>
       <c r="E5" t="n" s="5">
-        <v>0.04898958971218616</v>
+        <v>0.05389221556886228</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>13.788187446518148</v>
+        <v>14.95490439561841</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>15.083635392156648</v>
+        <v>15.819422484456974</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>-4.916364607843352</v>
+        <v>-11.180577515543026</v>
       </c>
     </row>
     <row r="6">
@@ -4288,19 +4288,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>24.0</v>
+        <v>31.0</v>
       </c>
       <c r="E6" t="n" s="5">
-        <v>0.05878750765462339</v>
+        <v>0.06187624750499002</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>23.124737186581623</v>
+        <v>23.860524278881947</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>-0.8752628134183773</v>
+        <v>-7.139475721118053</v>
       </c>
     </row>
     <row r="7">
@@ -4317,10 +4317,10 @@
         <v>12.0</v>
       </c>
       <c r="E7" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.023952095808383235</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>21.448291583472674</v>
+        <v>23.263184615406416</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>21.548050560223782</v>
@@ -4366,19 +4366,19 @@
         <v>0.036315615714757346</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>8.0</v>
+        <v>15.0</v>
       </c>
       <c r="E9" t="n" s="5">
-        <v>0.019595835884874464</v>
+        <v>0.029940119760479042</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>16.852229101299958</v>
+        <v>18.278216483533612</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>19.971363933865945</v>
+        <v>21.337825676709404</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>11.971363933865945</v>
+        <v>6.337825676709404</v>
       </c>
     </row>
     <row r="10">
@@ -4392,19 +4392,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="E10" t="n" s="5">
-        <v>0.0</v>
+        <v>0.013972055888223553</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>0.0</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>16.791712570710974</v>
+        <v>17.764002656964973</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>16.791712570710974</v>
+        <v>10.764002656964973</v>
       </c>
     </row>
     <row r="11">
@@ -4418,19 +4418,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>20.25</v>
+        <v>19.0</v>
       </c>
       <c r="E11" t="n" s="5">
-        <v>0.049601959583588484</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>18.526067859704593</v>
+        <v>19.025351958051242</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>-1.7239321402954069</v>
+        <v>0.025351958051242462</v>
       </c>
     </row>
     <row r="12">
@@ -4444,19 +4444,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="E12" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>13.788187446518148</v>
+        <v>14.95490439561841</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>19.708582829472974</v>
+        <v>21.49549433934519</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>7.708582829472974</v>
+        <v>2.495494339345189</v>
       </c>
     </row>
     <row r="13">
@@ -4470,19 +4470,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>24.0</v>
+        <v>31.0</v>
       </c>
       <c r="E13" t="n" s="5">
-        <v>0.05878750765462339</v>
+        <v>0.06187624750499002</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>18.38424992869086</v>
+        <v>19.93987252749121</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>24.175861604153514</v>
+        <v>25.121873579968216</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>0.17586160415351415</v>
+        <v>-5.8781264200317835</v>
       </c>
     </row>
     <row r="14">
@@ -4496,19 +4496,19 @@
         <v>0.05117200396170353</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>24.0</v>
+        <v>12.0</v>
       </c>
       <c r="E14" t="n" s="5">
-        <v>0.05878750765462339</v>
+        <v>0.023952095808383235</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>23.74632282455903</v>
+        <v>25.755668681342815</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>24.175861604153514</v>
+        <v>22.914512303067244</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>0.17586160415351415</v>
+        <v>10.914512303067244</v>
       </c>
     </row>
     <row r="15">
@@ -4548,19 +4548,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="E16" t="n" s="5">
-        <v>0.06858542559706063</v>
+        <v>0.05389221556886228</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>19.150260342386314</v>
+        <v>20.770700549470014</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>24.386086487667892</v>
+        <v>24.49119892942508</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>-3.6139135123321076</v>
+        <v>-2.5088010705749184</v>
       </c>
     </row>
     <row r="17">
@@ -4574,19 +4574,19 @@
         <v>0.034664905909541105</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="E17" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>16.086218687604507</v>
+        <v>17.447388461554812</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>19.23557684156562</v>
+        <v>20.181588817380323</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>7.235576841565621</v>
+        <v>1.181588817380323</v>
       </c>
     </row>
     <row r="18">
@@ -4600,19 +4600,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="E18" t="n" s="5">
-        <v>0.04898958971218616</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>19.23557684156562</v>
+        <v>19.34068928332281</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>-0.7644231584343792</v>
+        <v>0.3406892833228099</v>
       </c>
     </row>
     <row r="19">
@@ -4626,19 +4626,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D19" t="n" s="2">
-        <v>24.0</v>
+        <v>19.0</v>
       </c>
       <c r="E19" t="n" s="5">
-        <v>0.05878750765462339</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>20.759707247044865</v>
+        <v>20.444369921773298</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>-3.240292752955135</v>
+        <v>1.4443699217732977</v>
       </c>
     </row>
     <row r="20">
@@ -4652,19 +4652,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>24.0</v>
+        <v>31.0</v>
       </c>
       <c r="E20" t="n" s="5">
-        <v>0.05878750765462339</v>
+        <v>0.06187624750499002</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>18.38424992869086</v>
+        <v>19.93987252749121</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>23.334962070096</v>
+        <v>23.860524278881947</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>-0.665037929903999</v>
+        <v>-7.139475721118053</v>
       </c>
     </row>
     <row r="21">
@@ -4681,16 +4681,16 @@
         <v>20.0</v>
       </c>
       <c r="E21" t="n" s="5">
-        <v>0.04898958971218616</v>
+        <v>0.03992015968063872</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>21.448291583472674</v>
+        <v>23.263184615406416</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>25.016761138211027</v>
+        <v>24.386086487667892</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>5.016761138211027</v>
+        <v>4.386086487667892</v>
       </c>
     </row>
     <row r="22">
@@ -4730,19 +4730,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D23" t="n" s="2">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="E23" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>19.150260342386314</v>
+        <v>20.770700549470014</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>19.971363933865945</v>
+        <v>20.917375909680647</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>7.971363933865945</v>
+        <v>1.917375909680647</v>
       </c>
     </row>
     <row r="24">
@@ -4756,19 +4756,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D24" t="n" s="2">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="E24" t="n" s="5">
-        <v>0.0</v>
+        <v>0.013972055888223553</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>0.0</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G24" t="n" s="2">
-        <v>15.45152893830681</v>
+        <v>16.397540914121514</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>15.45152893830681</v>
+        <v>9.397540914121514</v>
       </c>
     </row>
     <row r="25">
@@ -4782,19 +4782,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D25" t="n" s="2">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>0.0</v>
+        <v>0.013972055888223553</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>0.0</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>15.766866263578379</v>
+        <v>16.71287823939308</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>15.766866263578379</v>
+        <v>9.712878239393081</v>
       </c>
     </row>
     <row r="26">
@@ -4808,19 +4808,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D26" t="n" s="2">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="E26" t="n" s="5">
-        <v>0.0</v>
+        <v>0.013972055888223553</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>0.0</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>18.86768329541546</v>
+        <v>19.813695271230163</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>18.86768329541546</v>
+        <v>12.813695271230163</v>
       </c>
     </row>
     <row r="27">
@@ -4834,19 +4834,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D27" t="n" s="2">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="E27" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>18.38424992869086</v>
+        <v>19.93987252749121</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>22.073612769009728</v>
+        <v>23.019624744824434</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>10.073612769009728</v>
+        <v>4.0196247448244335</v>
       </c>
     </row>
     <row r="28">
@@ -4863,16 +4863,16 @@
         <v>12.0</v>
       </c>
       <c r="E28" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.023952095808383235</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>21.448291583472674</v>
+        <v>23.263184615406416</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>23.755411837124758</v>
+        <v>23.334962070096</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>11.755411837124758</v>
+        <v>11.334962070096001</v>
       </c>
     </row>
     <row r="29">
@@ -4912,19 +4912,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D30" t="n" s="2">
-        <v>24.0</v>
+        <v>31.0</v>
       </c>
       <c r="E30" t="n" s="5">
-        <v>0.05878750765462339</v>
+        <v>0.06187624750499002</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>19.150260342386314</v>
+        <v>20.770700549470014</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>20.917375909680647</v>
+        <v>22.073612769009728</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>-3.082624090319353</v>
+        <v>-8.926387230990272</v>
       </c>
     </row>
     <row r="31">
@@ -4938,19 +4938,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D31" t="n" s="2">
-        <v>12.0</v>
+        <v>7.0</v>
       </c>
       <c r="E31" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.013972055888223553</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>18.710014632779675</v>
+        <v>18.394677307508108</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>6.710014632779675</v>
+        <v>11.394677307508108</v>
       </c>
     </row>
     <row r="32">
@@ -4964,19 +4964,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D32" t="n" s="2">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="E32" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>18.604902191022486</v>
+        <v>19.550914166837188</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>6.604902191022486</v>
+        <v>0.5509141668371882</v>
       </c>
     </row>
     <row r="33">
@@ -4990,19 +4990,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D33" t="n" s="2">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="E33" t="n" s="5">
-        <v>0.029393753827311696</v>
+        <v>0.03792415169660679</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>15.320208273909051</v>
+        <v>16.616560439576006</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>20.02392015474454</v>
+        <v>20.969932130559243</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>8.023920154744541</v>
+        <v>1.9699321305592434</v>
       </c>
     </row>
     <row r="34">
@@ -5016,19 +5016,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D34" t="n" s="2">
-        <v>20.0</v>
+        <v>27.0</v>
       </c>
       <c r="E34" t="n" s="5">
-        <v>0.04898958971218616</v>
+        <v>0.05389221556886228</v>
       </c>
       <c r="F34" t="n" s="2">
-        <v>18.38424992869086</v>
+        <v>19.93987252749121</v>
       </c>
       <c r="G34" t="n" s="2">
-        <v>20.70715102616627</v>
+        <v>22.494062536038488</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>0.7071510261662688</v>
+        <v>-4.505937463961512</v>
       </c>
     </row>
     <row r="35">
@@ -5042,19 +5042,19 @@
         <v>1.0</v>
       </c>
       <c r="D35" t="n" s="3">
-        <v>408.25</v>
+        <v>501.0</v>
       </c>
       <c r="E35" t="n" s="3">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="3">
-        <v>400.62344636272167</v>
+        <v>500.9892972532167</v>
       </c>
       <c r="G35" t="n" s="3">
-        <v>547.7934902175914</v>
+        <v>563.0347942723839</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>139.5434902175914</v>
+        <v>62.03479427238392</v>
       </c>
     </row>
     <row r="36">
@@ -5152,16 +5152,16 @@
         <v>30.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>0.031880977683315624</v>
+        <v>0.02827521206409048</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>28.08895216821741</v>
+        <v>31.67096519710805</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>18.691751943413426</v>
+        <v>18.58180046139335</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>-11.308248056586574</v>
+        <v>-11.41819953860665</v>
       </c>
     </row>
     <row r="5">
@@ -5178,16 +5178,16 @@
         <v>23.0</v>
       </c>
       <c r="E5" t="n" s="5">
-        <v>0.024442082890541977</v>
+        <v>0.021677662582469368</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>28.08895216821741</v>
+        <v>31.67096519710805</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>15.778037669881334</v>
+        <v>16.547698044021885</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>-7.221962330118666</v>
+        <v>-6.452301955978115</v>
       </c>
     </row>
     <row r="6">
@@ -5204,16 +5204,16 @@
         <v>38.0</v>
       </c>
       <c r="E6" t="n" s="5">
-        <v>0.040382571732199786</v>
+        <v>0.03581526861451461</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>24.189326044417378</v>
+        <v>24.95898641855793</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>-13.810673955582622</v>
+        <v>-13.04101358144207</v>
       </c>
     </row>
     <row r="7">
@@ -5230,10 +5230,10 @@
         <v>34.0</v>
       </c>
       <c r="E7" t="n" s="5">
-        <v>0.036131774707757705</v>
+        <v>0.03204524033930255</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>43.69392559500486</v>
+        <v>49.26594586216808</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>22.54005381411619</v>
@@ -5279,19 +5279,19 @@
         <v>0.036315615714757346</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="E9" t="n" s="5">
-        <v>0.04144527098831031</v>
+        <v>0.04241281809613572</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>34.33094153893239</v>
+        <v>38.70895746313206</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>20.890781583815006</v>
+        <v>22.320150850076033</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>-18.109218416184994</v>
+        <v>-22.679849149923967</v>
       </c>
     </row>
     <row r="10">
@@ -5305,19 +5305,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>35.0</v>
+        <v>41.0</v>
       </c>
       <c r="E10" t="n" s="5">
-        <v>0.03719447396386823</v>
+        <v>0.03864278982092366</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>17.564749252707617</v>
+        <v>18.58180046139335</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>-17.435250747292383</v>
+        <v>-22.41819953860665</v>
       </c>
     </row>
     <row r="11">
@@ -5331,19 +5331,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>38.0</v>
+        <v>44.0</v>
       </c>
       <c r="E11" t="n" s="5">
-        <v>0.040382571732199786</v>
+        <v>0.04147031102733271</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>19.37894870603892</v>
+        <v>19.901218245634297</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>-18.62105129396108</v>
+        <v>-24.098781754365703</v>
       </c>
     </row>
     <row r="12">
@@ -5357,19 +5357,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>32.0</v>
+        <v>38.0</v>
       </c>
       <c r="E12" t="n" s="5">
-        <v>0.03400637619553666</v>
+        <v>0.03581526861451461</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>28.08895216821741</v>
+        <v>31.67096519710805</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>20.61590287876481</v>
+        <v>22.485078073106152</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>-11.38409712123519</v>
+        <v>-15.514921926893848</v>
       </c>
     </row>
     <row r="13">
@@ -5383,19 +5383,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>38.0</v>
+        <v>44.0</v>
       </c>
       <c r="E13" t="n" s="5">
-        <v>0.040382571732199786</v>
+        <v>0.04147031102733271</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>37.45193622428988</v>
+        <v>42.22795359614406</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>25.288840864618166</v>
+        <v>26.27840420279888</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>-12.711159135381834</v>
+        <v>-17.72159579720112</v>
       </c>
     </row>
     <row r="14">
@@ -5412,16 +5412,16 @@
         <v>29.0</v>
       </c>
       <c r="E14" t="n" s="5">
-        <v>0.030818278427205102</v>
+        <v>0.027332704995287466</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>48.375417623041095</v>
+        <v>54.54444006168608</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>25.288840864618166</v>
+        <v>23.96942308037722</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>-3.711159135381834</v>
+        <v>-5.030576919622781</v>
       </c>
     </row>
     <row r="15">
@@ -5461,19 +5461,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="E16" t="n" s="5">
-        <v>0.04144527098831031</v>
+        <v>0.04241281809613572</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>39.01243356696863</v>
+        <v>43.987451662650074</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>25.508743828658325</v>
+        <v>25.618695310678405</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>-13.491256171341675</v>
+        <v>-19.381304689321595</v>
       </c>
     </row>
     <row r="17">
@@ -5487,19 +5487,19 @@
         <v>0.034664905909541105</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>36.0</v>
+        <v>42.0</v>
       </c>
       <c r="E17" t="n" s="5">
-        <v>0.03825717321997875</v>
+        <v>0.03958529688972667</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>32.77044419625365</v>
+        <v>36.94945939662606</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>20.121121209674453</v>
+        <v>21.110684547855165</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>-15.878878790325547</v>
+        <v>-20.889315452144835</v>
       </c>
     </row>
     <row r="18">
@@ -5513,19 +5513,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>37.0</v>
+        <v>43.0</v>
       </c>
       <c r="E18" t="n" s="5">
-        <v>0.039319872476089264</v>
+        <v>0.04052780395852969</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>20.121121209674453</v>
+        <v>20.231072691694532</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>-16.878878790325547</v>
+        <v>-22.768927308305468</v>
       </c>
     </row>
     <row r="19">
@@ -5539,19 +5539,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D19" t="n" s="2">
-        <v>36.0</v>
+        <v>42.0</v>
       </c>
       <c r="E19" t="n" s="5">
-        <v>0.03825717321997875</v>
+        <v>0.03958529688972667</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>21.7154176989656</v>
+        <v>21.385563252905364</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>-14.284582301034401</v>
+        <v>-20.614436747094636</v>
       </c>
     </row>
     <row r="20">
@@ -5565,19 +5565,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="E20" t="n" s="5">
-        <v>0.04250797024442083</v>
+        <v>0.043355325164938736</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>37.45193622428988</v>
+        <v>42.22795359614406</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>24.409229008457533</v>
+        <v>24.95898641855793</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>-15.590770991542467</v>
+        <v>-21.04101358144207</v>
       </c>
     </row>
     <row r="21">
@@ -5594,16 +5594,16 @@
         <v>36.0</v>
       </c>
       <c r="E21" t="n" s="5">
-        <v>0.03825717321997875</v>
+        <v>0.033930254476908575</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>43.69392559500486</v>
+        <v>49.26594586216808</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>26.1684527207788</v>
+        <v>25.508743828658325</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>-9.831547279221201</v>
+        <v>-10.491256171341675</v>
       </c>
     </row>
     <row r="22">
@@ -5643,19 +5643,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D23" t="n" s="2">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="E23" t="n" s="5">
-        <v>0.04144527098831031</v>
+        <v>0.04241281809613572</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>39.01243356696863</v>
+        <v>43.987451662650074</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>20.890781583815006</v>
+        <v>21.880344921995718</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>-18.109218416184994</v>
+        <v>-23.119655078004282</v>
       </c>
     </row>
     <row r="24">
@@ -5669,19 +5669,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D24" t="n" s="2">
-        <v>30.0</v>
+        <v>36.0</v>
       </c>
       <c r="E24" t="n" s="5">
-        <v>0.031880977683315624</v>
+        <v>0.033930254476908575</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G24" t="n" s="2">
-        <v>16.16286785695161</v>
+        <v>17.152431195132323</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>-13.83713214304839</v>
+        <v>-18.847568804867677</v>
       </c>
     </row>
     <row r="25">
@@ -5695,19 +5695,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D25" t="n" s="2">
-        <v>23.0</v>
+        <v>29.0</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>0.024442082890541977</v>
+        <v>0.027332704995287466</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>16.49272230301185</v>
+        <v>17.482285641192558</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>-6.507277696988151</v>
+        <v>-11.517714358807442</v>
       </c>
     </row>
     <row r="26">
@@ -5721,19 +5721,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D26" t="n" s="2">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="E26" t="n" s="5">
-        <v>0.04144527098831031</v>
+        <v>0.04241281809613572</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>19.736291022604178</v>
+        <v>20.72585436078489</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>-19.263708977395822</v>
+        <v>-24.27414563921511</v>
       </c>
     </row>
     <row r="27">
@@ -5747,19 +5747,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D27" t="n" s="2">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="E27" t="n" s="5">
-        <v>0.04250797024442083</v>
+        <v>0.043355325164938736</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>37.45193622428988</v>
+        <v>42.22795359614406</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>23.089811224216586</v>
+        <v>24.079374562397298</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>-16.910188775783414</v>
+        <v>-21.920625437602702</v>
       </c>
     </row>
     <row r="28">
@@ -5776,16 +5776,16 @@
         <v>32.0</v>
       </c>
       <c r="E28" t="n" s="5">
-        <v>0.03400637619553666</v>
+        <v>0.030160226201696512</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>43.69392559500486</v>
+        <v>49.26594586216808</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>24.84903493653785</v>
+        <v>24.409229008457533</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>-7.150965063462149</v>
+        <v>-7.590770991542467</v>
       </c>
     </row>
     <row r="29">
@@ -5825,19 +5825,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D30" t="n" s="2">
-        <v>32.0</v>
+        <v>38.0</v>
       </c>
       <c r="E30" t="n" s="5">
-        <v>0.03400637619553666</v>
+        <v>0.03581526861451461</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>39.01243356696863</v>
+        <v>43.987451662650074</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>21.880344921995718</v>
+        <v>23.089811224216586</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>-10.119655078004282</v>
+        <v>-14.910188775783414</v>
       </c>
     </row>
     <row r="31">
@@ -5851,19 +5851,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D31" t="n" s="2">
-        <v>37.0</v>
+        <v>43.0</v>
       </c>
       <c r="E31" t="n" s="5">
-        <v>0.039319872476089264</v>
+        <v>0.04052780395852969</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>19.57136379957406</v>
+        <v>19.241509353513823</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>-17.42863620042594</v>
+        <v>-23.758490646486177</v>
       </c>
     </row>
     <row r="32">
@@ -5877,19 +5877,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D32" t="n" s="2">
-        <v>30.0</v>
+        <v>36.0</v>
       </c>
       <c r="E32" t="n" s="5">
-        <v>0.031880977683315624</v>
+        <v>0.033930254476908575</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>19.46141231755398</v>
+        <v>20.45097565573469</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>-10.538587682446021</v>
+        <v>-15.549024344265309</v>
       </c>
     </row>
     <row r="33">
@@ -5903,19 +5903,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D33" t="n" s="2">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="E33" t="n" s="5">
-        <v>0.04144527098831031</v>
+        <v>0.04241281809613572</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>31.209946853574895</v>
+        <v>35.18996133012005</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>20.945757324825045</v>
+        <v>21.935320663005758</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>-18.054242675174955</v>
+        <v>-23.064679336994242</v>
       </c>
     </row>
     <row r="34">
@@ -5929,19 +5929,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D34" t="n" s="2">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="E34" t="n" s="5">
-        <v>0.04250797024442083</v>
+        <v>0.043355325164938736</v>
       </c>
       <c r="F34" t="n" s="2">
-        <v>37.45193622428988</v>
+        <v>42.22795359614406</v>
       </c>
       <c r="G34" t="n" s="2">
-        <v>21.66044195795556</v>
+        <v>23.529617152296904</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>-18.33955804204444</v>
+        <v>-22.470382847703096</v>
       </c>
     </row>
     <row r="35">
@@ -5955,19 +5955,19 @@
         <v>1.0</v>
       </c>
       <c r="D35" t="n" s="3">
-        <v>941.0</v>
+        <v>1061.0</v>
       </c>
       <c r="E35" t="n" s="3">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="3">
-        <v>940.9798976352835</v>
+        <v>1060.9773341031196</v>
       </c>
       <c r="G35" t="n" s="3">
-        <v>573.0121485476416</v>
+        <v>588.9551134405531</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>-367.9878514523584</v>
+        <v>-472.0448865594469</v>
       </c>
     </row>
     <row r="36">
@@ -6065,16 +6065,16 @@
         <v>29.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>0.026268115942028984</v>
+        <v>0.027992277992277992</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>32.95451986579386</v>
+        <v>30.924712482755833</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>27.680915091772558</v>
+        <v>27.518086179468014</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>-1.3190849082274418</v>
+        <v>-1.481913820531986</v>
       </c>
     </row>
     <row r="5">
@@ -6091,16 +6091,16 @@
         <v>27.0</v>
       </c>
       <c r="E5" t="n" s="5">
-        <v>0.024456521739130436</v>
+        <v>0.026061776061776062</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>32.95451986579386</v>
+        <v>30.924712482755833</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>23.36594891570213</v>
+        <v>24.505751301833943</v>
       </c>
       <c r="H5" t="n" s="2">
-        <v>-3.6340510842978695</v>
+        <v>-2.494248698166057</v>
       </c>
     </row>
     <row r="6">
@@ -6117,16 +6117,16 @@
         <v>43.0</v>
       </c>
       <c r="E6" t="n" s="5">
-        <v>0.03894927536231884</v>
+        <v>0.041505791505791506</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>35.82236070699978</v>
+        <v>36.96216309313159</v>
       </c>
       <c r="H6" t="n" s="2">
-        <v>-7.177639293000219</v>
+        <v>-6.037836906868407</v>
       </c>
     </row>
     <row r="7">
@@ -6143,10 +6143,10 @@
         <v>53.0</v>
       </c>
       <c r="E7" t="n" s="5">
-        <v>0.04800724637681159</v>
+        <v>0.05115830115830116</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>51.26258645790156</v>
+        <v>48.105108306509074</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>33.379927022431616</v>
@@ -6195,16 +6195,16 @@
         <v>39.0</v>
       </c>
       <c r="E9" t="n" s="5">
-        <v>0.035326086956521736</v>
+        <v>0.037644787644787646</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>40.27774650263694</v>
+        <v>37.796870812257126</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>30.937493337863447</v>
+        <v>33.05426919782253</v>
       </c>
       <c r="H9" t="n" s="2">
-        <v>-8.062506662136553</v>
+        <v>-5.945730802177472</v>
       </c>
     </row>
     <row r="10">
@@ -6221,16 +6221,16 @@
         <v>23.0</v>
       </c>
       <c r="E10" t="n" s="5">
-        <v>0.020833333333333332</v>
+        <v>0.0222007722007722</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>26.011918740650977</v>
+        <v>27.518086179468014</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>3.0119187406509766</v>
+        <v>4.518086179468014</v>
       </c>
     </row>
     <row r="11">
@@ -6247,16 +6247,16 @@
         <v>24.0</v>
       </c>
       <c r="E11" t="n" s="5">
-        <v>0.021739130434782608</v>
+        <v>0.023166023166023165</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>28.698595793675963</v>
+        <v>29.472033127122547</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>4.698595793675963</v>
+        <v>5.472033127122547</v>
       </c>
     </row>
     <row r="12">
@@ -6270,19 +6270,19 @@
         <v>0.029712776493892375</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>47.0</v>
+        <v>43.0</v>
       </c>
       <c r="E12" t="n" s="5">
-        <v>0.042572463768115944</v>
+        <v>0.041505791505791506</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>32.95451986579386</v>
+        <v>30.924712482755833</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>30.53042105710209</v>
+        <v>33.29851256627934</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>-16.46957894289791</v>
+        <v>-9.701487433720658</v>
       </c>
     </row>
     <row r="13">
@@ -6296,19 +6296,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>63.0</v>
+        <v>59.0</v>
       </c>
       <c r="E13" t="n" s="5">
-        <v>0.057065217391304345</v>
+        <v>0.05694980694980695</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>43.939359821058474</v>
+        <v>41.23294997700777</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>37.45064983004523</v>
+        <v>38.91611004078613</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>-25.54935016995477</v>
+        <v>-20.08388995921387</v>
       </c>
     </row>
     <row r="14">
@@ -6325,16 +6325,16 @@
         <v>57.0</v>
       </c>
       <c r="E14" t="n" s="5">
-        <v>0.051630434782608696</v>
+        <v>0.05501930501930502</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>56.755006435533865</v>
+        <v>53.259227053635044</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>37.45064983004523</v>
+        <v>35.49670288239069</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>-19.54935016995477</v>
+        <v>-21.503297117609307</v>
       </c>
     </row>
     <row r="15">
@@ -6374,19 +6374,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>41.0</v>
+        <v>37.0</v>
       </c>
       <c r="E16" t="n" s="5">
-        <v>0.03713768115942029</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>45.77016648026925</v>
+        <v>42.9509895593831</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>37.77630765465432</v>
+        <v>37.93913656695886</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>-3.2236923453456825</v>
+        <v>0.939136566958858</v>
       </c>
     </row>
     <row r="17">
@@ -6400,19 +6400,19 @@
         <v>0.034664905909541105</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>35.0</v>
+        <v>31.0</v>
       </c>
       <c r="E17" t="n" s="5">
-        <v>0.03170289855072464</v>
+        <v>0.029922779922779922</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>38.44693984342617</v>
+        <v>36.07883122988181</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>29.79769095173164</v>
+        <v>31.26315116247254</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>-5.202309048268361</v>
+        <v>0.2631511624725391</v>
       </c>
     </row>
     <row r="18">
@@ -6426,19 +6426,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E18" t="n" s="5">
-        <v>0.03260869565217391</v>
+        <v>0.03088803088803089</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>29.79769095173164</v>
+        <v>29.960519864036183</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>-6.202309048268361</v>
+        <v>-2.0394801359638173</v>
       </c>
     </row>
     <row r="19">
@@ -6452,19 +6452,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D19" t="n" s="2">
-        <v>39.0</v>
+        <v>35.0</v>
       </c>
       <c r="E19" t="n" s="5">
-        <v>0.035326086956521736</v>
+        <v>0.033783783783783786</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>32.15871018014753</v>
+        <v>31.670223443233898</v>
       </c>
       <c r="H19" t="n" s="2">
-        <v>-6.84128981985247</v>
+        <v>-3.3297765567661024</v>
       </c>
     </row>
     <row r="20">
@@ -6478,19 +6478,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>59.0</v>
+        <v>55.0</v>
       </c>
       <c r="E20" t="n" s="5">
-        <v>0.05344202898550725</v>
+        <v>0.05308880308880309</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>43.939359821058474</v>
+        <v>41.23294997700777</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>36.14801853160887</v>
+        <v>36.96216309313159</v>
       </c>
       <c r="H20" t="n" s="2">
-        <v>-22.85198146839113</v>
+        <v>-18.037836906868407</v>
       </c>
     </row>
     <row r="21">
@@ -6507,16 +6507,16 @@
         <v>45.0</v>
       </c>
       <c r="E21" t="n" s="5">
-        <v>0.04076086956521739</v>
+        <v>0.04343629343629344</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>51.26258645790156</v>
+        <v>48.105108306509074</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>38.75328112848158</v>
+        <v>37.77630765465432</v>
       </c>
       <c r="H21" t="n" s="2">
-        <v>-6.246718871518418</v>
+        <v>-7.2236923453456825</v>
       </c>
     </row>
     <row r="22">
@@ -6556,19 +6556,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D23" t="n" s="2">
-        <v>33.0</v>
+        <v>29.0</v>
       </c>
       <c r="E23" t="n" s="5">
-        <v>0.029891304347826088</v>
+        <v>0.027992277992277992</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>45.77016648026925</v>
+        <v>42.9509895593831</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>30.937493337863447</v>
+        <v>32.40295354860435</v>
       </c>
       <c r="H23" t="n" s="2">
-        <v>-2.0625066621365526</v>
+        <v>3.4029535486043514</v>
       </c>
     </row>
     <row r="24">
@@ -6582,19 +6582,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D24" t="n" s="2">
-        <v>27.0</v>
+        <v>23.0</v>
       </c>
       <c r="E24" t="n" s="5">
-        <v>0.024456521739130436</v>
+        <v>0.0222007722007722</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G24" t="n" s="2">
-        <v>23.935850108768037</v>
+        <v>25.401310319508937</v>
       </c>
       <c r="H24" t="n" s="2">
-        <v>-3.0641498912319634</v>
+        <v>2.401310319508937</v>
       </c>
     </row>
     <row r="25">
@@ -6608,19 +6608,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D25" t="n" s="2">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>0.03260869565217391</v>
+        <v>0.03088803088803089</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>24.42433684568167</v>
+        <v>25.88979705642257</v>
       </c>
       <c r="H25" t="n" s="2">
-        <v>-11.575663154318331</v>
+        <v>-6.1102029435774305</v>
       </c>
     </row>
     <row r="26">
@@ -6634,19 +6634,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D26" t="n" s="2">
-        <v>47.0</v>
+        <v>43.0</v>
       </c>
       <c r="E26" t="n" s="5">
-        <v>0.042572463768115944</v>
+        <v>0.041505791505791506</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>29.227789758665732</v>
+        <v>30.693249969406633</v>
       </c>
       <c r="H26" t="n" s="2">
-        <v>-17.772210241334268</v>
+        <v>-12.306750030593367</v>
       </c>
     </row>
     <row r="27">
@@ -6660,19 +6660,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D27" t="n" s="2">
-        <v>59.0</v>
+        <v>55.0</v>
       </c>
       <c r="E27" t="n" s="5">
-        <v>0.05344202898550725</v>
+        <v>0.05308880308880309</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>43.939359821058474</v>
+        <v>41.23294997700777</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>34.19407158395434</v>
+        <v>35.65953179469524</v>
       </c>
       <c r="H27" t="n" s="2">
-        <v>-24.80592841604566</v>
+        <v>-19.34046820530476</v>
       </c>
     </row>
     <row r="28">
@@ -6689,16 +6689,16 @@
         <v>61.0</v>
       </c>
       <c r="E28" t="n" s="5">
-        <v>0.0552536231884058</v>
+        <v>0.05888030888030888</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>51.26258645790156</v>
+        <v>48.105108306509074</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>36.799334180827046</v>
+        <v>36.14801853160887</v>
       </c>
       <c r="H28" t="n" s="2">
-        <v>-24.200665819172954</v>
+        <v>-24.85198146839113</v>
       </c>
     </row>
     <row r="29">
@@ -6738,19 +6738,19 @@
         <v>0.041267745130406076</v>
       </c>
       <c r="D30" t="n" s="2">
-        <v>35.0</v>
+        <v>31.0</v>
       </c>
       <c r="E30" t="n" s="5">
-        <v>0.03170289855072464</v>
+        <v>0.029922779922779922</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>45.77016648026925</v>
+        <v>42.9509895593831</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>32.40295354860435</v>
+        <v>34.19407158395434</v>
       </c>
       <c r="H30" t="n" s="2">
-        <v>-2.5970464513956486</v>
+        <v>3.19407158395434</v>
       </c>
     </row>
     <row r="31">
@@ -6764,19 +6764,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D31" t="n" s="2">
-        <v>35.0</v>
+        <v>31.0</v>
       </c>
       <c r="E31" t="n" s="5">
-        <v>0.03170289855072464</v>
+        <v>0.029922779922779922</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>28.983546390208915</v>
+        <v>28.495059653295282</v>
       </c>
       <c r="H31" t="n" s="2">
-        <v>-6.0164536097910855</v>
+        <v>-2.5049403467047178</v>
       </c>
     </row>
     <row r="32">
@@ -6790,19 +6790,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D32" t="n" s="2">
-        <v>33.0</v>
+        <v>29.0</v>
       </c>
       <c r="E32" t="n" s="5">
-        <v>0.029891304347826088</v>
+        <v>0.027992277992277992</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>28.82071747790437</v>
+        <v>30.28617768864527</v>
       </c>
       <c r="H32" t="n" s="2">
-        <v>-4.17928252209563</v>
+        <v>1.286177688645271</v>
       </c>
     </row>
     <row r="33">
@@ -6816,19 +6816,19 @@
         <v>0.03301419610432486</v>
       </c>
       <c r="D33" t="n" s="2">
-        <v>39.0</v>
+        <v>35.0</v>
       </c>
       <c r="E33" t="n" s="5">
-        <v>0.035326086956521736</v>
+        <v>0.033783783783783786</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>36.61613318421539</v>
+        <v>34.360791647506474</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>31.01890779401572</v>
+        <v>32.48436800475662</v>
       </c>
       <c r="H33" t="n" s="2">
-        <v>-7.981092205984279</v>
+        <v>-2.515631995243382</v>
       </c>
     </row>
     <row r="34">
@@ -6842,19 +6842,19 @@
         <v>0.03961703532518983</v>
       </c>
       <c r="D34" t="n" s="2">
-        <v>39.0</v>
+        <v>35.0</v>
       </c>
       <c r="E34" t="n" s="5">
-        <v>0.035326086956521736</v>
+        <v>0.033783783783783786</v>
       </c>
       <c r="F34" t="n" s="2">
-        <v>43.939359821058474</v>
+        <v>41.23294997700777</v>
       </c>
       <c r="G34" t="n" s="2">
-        <v>32.07729572399526</v>
+        <v>34.84538723317252</v>
       </c>
       <c r="H34" t="n" s="2">
-        <v>-6.922704276004737</v>
+        <v>-0.15461276682748348</v>
       </c>
     </row>
     <row r="35">
@@ -6868,19 +6868,19 @@
         <v>1.0</v>
       </c>
       <c r="D35" t="n" s="3">
-        <v>1104.0</v>
+        <v>1036.0</v>
       </c>
       <c r="E35" t="n" s="3">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="3">
-        <v>1103.9764155040943</v>
+        <v>1035.9778681723205</v>
       </c>
       <c r="G35" t="n" s="3">
-        <v>848.5828764751335</v>
+        <v>872.1930687592924</v>
       </c>
       <c r="H35" t="n" s="3">
-        <v>-255.4171235248665</v>
+        <v>-163.80693124070763</v>
       </c>
     </row>
     <row r="36">

</xml_diff>